<commit_message>
menambah daftar nilai di Hlookup
</commit_message>
<xml_diff>
--- a/LATIHAN EXCEL AHMADI.xlsx
+++ b/LATIHAN EXCEL AHMADI.xlsx
@@ -9,24 +9,29 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="13335" windowHeight="5130" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="13335" windowHeight="5130" firstSheet="5" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="RPBMK FISTAN FISTUM" sheetId="4" r:id="rId1"/>
     <sheet name="ALOKASI waktu" sheetId="7" r:id="rId2"/>
-    <sheet name="coba reference" sheetId="5" r:id="rId3"/>
-    <sheet name="RAB SDC" sheetId="8" r:id="rId4"/>
+    <sheet name="RAB SDC" sheetId="8" r:id="rId3"/>
+    <sheet name="daftar harga" sheetId="9" r:id="rId4"/>
+    <sheet name="kegiatan1" sheetId="5" r:id="rId5"/>
+    <sheet name="kegiatan 2" sheetId="12" r:id="rId6"/>
+    <sheet name="kegiatan 3" sheetId="14" r:id="rId7"/>
+    <sheet name="kegiatan 4" sheetId="15" r:id="rId8"/>
+    <sheet name="penentuan baju" sheetId="13" r:id="rId9"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId5"/>
-    <externalReference r:id="rId6"/>
+    <externalReference r:id="rId10"/>
+    <externalReference r:id="rId11"/>
   </externalReferences>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="199">
   <si>
     <t>Satuan</t>
   </si>
@@ -220,9 +225,6 @@
     <t>Aqua gelas</t>
   </si>
   <si>
-    <t>Aqua Galon</t>
-  </si>
-  <si>
     <t>Tisue</t>
   </si>
   <si>
@@ -298,9 +300,6 @@
     <t>Ujian</t>
   </si>
   <si>
-    <t>RENCANA PROGRAM PEMBELAJARAN DIKLAT  SDC</t>
-  </si>
-  <si>
     <t>Paket</t>
   </si>
   <si>
@@ -485,6 +484,150 @@
   </si>
   <si>
     <t>NIP. 19860505 201403 1 003</t>
+  </si>
+  <si>
+    <t>RENCANA KEGIATAN PELATIHAN</t>
+  </si>
+  <si>
+    <t>galon</t>
+  </si>
+  <si>
+    <t>Kegiatan 1</t>
+  </si>
+  <si>
+    <t>Ketua Panitia,</t>
+  </si>
+  <si>
+    <t>Ahmadi Muslim</t>
+  </si>
+  <si>
+    <t>Nip. 81376481273681</t>
+  </si>
+  <si>
+    <t>Transport</t>
+  </si>
+  <si>
+    <t>Honor</t>
+  </si>
+  <si>
+    <t>senin</t>
+  </si>
+  <si>
+    <t>selasa</t>
+  </si>
+  <si>
+    <t>rabu</t>
+  </si>
+  <si>
+    <t>kamis</t>
+  </si>
+  <si>
+    <t>jumat</t>
+  </si>
+  <si>
+    <t>sabtu</t>
+  </si>
+  <si>
+    <t>Hari</t>
+  </si>
+  <si>
+    <t>Putih abu</t>
+  </si>
+  <si>
+    <t>Batik</t>
+  </si>
+  <si>
+    <t>Praktik</t>
+  </si>
+  <si>
+    <t>Pramuka</t>
+  </si>
+  <si>
+    <t>Olahraga</t>
+  </si>
+  <si>
+    <t>Baju Siswa</t>
+  </si>
+  <si>
+    <t>Baju Guru</t>
+  </si>
+  <si>
+    <t>PDH</t>
+  </si>
+  <si>
+    <t>Putih hitam</t>
+  </si>
+  <si>
+    <t>Adat</t>
+  </si>
+  <si>
+    <t>Bebas</t>
+  </si>
+  <si>
+    <t>kegiatan1</t>
+  </si>
+  <si>
+    <t>kegiatan2</t>
+  </si>
+  <si>
+    <t>kegiatan3</t>
+  </si>
+  <si>
+    <t>kegiatan4</t>
+  </si>
+  <si>
+    <t>kegiatan5</t>
+  </si>
+  <si>
+    <t>kegiatan6</t>
+  </si>
+  <si>
+    <t>kegiatan7</t>
+  </si>
+  <si>
+    <t>kegiatan8</t>
+  </si>
+  <si>
+    <t>kegiatan9</t>
+  </si>
+  <si>
+    <t>kegiatan10</t>
+  </si>
+  <si>
+    <t>kegiatan11</t>
+  </si>
+  <si>
+    <t>kegiatan12</t>
+  </si>
+  <si>
+    <t>kegiatan13</t>
+  </si>
+  <si>
+    <t>kegiatan14</t>
+  </si>
+  <si>
+    <t>kegiatan15</t>
+  </si>
+  <si>
+    <t>kegiatan16</t>
+  </si>
+  <si>
+    <t>kegiatan17</t>
+  </si>
+  <si>
+    <t>kegiatan18</t>
+  </si>
+  <si>
+    <t>kegiatan19</t>
+  </si>
+  <si>
+    <t>kegiatan20</t>
+  </si>
+  <si>
+    <t>kegiatan21</t>
+  </si>
+  <si>
+    <t>Kegiatan</t>
   </si>
 </sst>
 </file>
@@ -496,7 +639,7 @@
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -602,6 +745,14 @@
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -723,7 +874,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -875,39 +1026,12 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -923,15 +1047,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -943,12 +1058,6 @@
     </xf>
     <xf numFmtId="3" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -993,6 +1102,65 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1358,10 +1526,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="1"/>
+  </sheetPr>
   <dimension ref="A1:M93"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1382,58 +1553,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="82" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55" t="s">
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
+      <c r="F1" s="82"/>
+      <c r="G1" s="82" t="s">
         <v>58</v>
       </c>
-      <c r="H1" s="55"/>
-      <c r="I1" s="55"/>
-      <c r="J1" s="55"/>
-      <c r="K1" s="55"/>
-      <c r="L1" s="55"/>
+      <c r="H1" s="82"/>
+      <c r="I1" s="82"/>
+      <c r="J1" s="82"/>
+      <c r="K1" s="82"/>
+      <c r="L1" s="82"/>
     </row>
     <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="82" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="55"/>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55" t="s">
+      <c r="B2" s="82"/>
+      <c r="C2" s="82"/>
+      <c r="D2" s="82"/>
+      <c r="E2" s="82"/>
+      <c r="F2" s="82"/>
+      <c r="G2" s="82" t="s">
         <v>36</v>
       </c>
-      <c r="H2" s="55"/>
-      <c r="I2" s="55"/>
-      <c r="J2" s="55"/>
-      <c r="K2" s="55"/>
-      <c r="L2" s="55"/>
+      <c r="H2" s="82"/>
+      <c r="I2" s="82"/>
+      <c r="J2" s="82"/>
+      <c r="K2" s="82"/>
+      <c r="L2" s="82"/>
     </row>
     <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="82" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="55"/>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="55"/>
-      <c r="G3" s="55" t="s">
+      <c r="B3" s="82"/>
+      <c r="C3" s="82"/>
+      <c r="D3" s="82"/>
+      <c r="E3" s="82"/>
+      <c r="F3" s="82"/>
+      <c r="G3" s="82" t="s">
         <v>35</v>
       </c>
-      <c r="H3" s="55"/>
-      <c r="I3" s="55"/>
-      <c r="J3" s="55"/>
-      <c r="K3" s="55"/>
-      <c r="L3" s="55"/>
+      <c r="H3" s="82"/>
+      <c r="I3" s="82"/>
+      <c r="J3" s="82"/>
+      <c r="K3" s="82"/>
+      <c r="L3" s="82"/>
     </row>
     <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E4" s="1"/>
@@ -1442,14 +1613,14 @@
       <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="56" t="s">
+      <c r="A6" s="81" t="s">
         <v>57</v>
       </c>
-      <c r="B6" s="56"/>
-      <c r="C6" s="56"/>
-      <c r="D6" s="56"/>
-      <c r="E6" s="56"/>
-      <c r="F6" s="56"/>
+      <c r="B6" s="81"/>
+      <c r="C6" s="81"/>
+      <c r="D6" s="81"/>
+      <c r="E6" s="81"/>
+      <c r="F6" s="81"/>
       <c r="G6" s="20" t="s">
         <v>4</v>
       </c>
@@ -2871,61 +3042,61 @@
       <c r="L61" s="11"/>
     </row>
     <row r="62" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="55" t="s">
+      <c r="A62" s="82" t="s">
         <v>38</v>
       </c>
-      <c r="B62" s="55"/>
-      <c r="C62" s="55"/>
-      <c r="D62" s="55"/>
-      <c r="E62" s="55"/>
-      <c r="F62" s="55"/>
-      <c r="G62" s="55" t="s">
+      <c r="B62" s="82"/>
+      <c r="C62" s="82"/>
+      <c r="D62" s="82"/>
+      <c r="E62" s="82"/>
+      <c r="F62" s="82"/>
+      <c r="G62" s="82" t="s">
         <v>37</v>
       </c>
-      <c r="H62" s="55"/>
-      <c r="I62" s="55"/>
-      <c r="J62" s="55"/>
-      <c r="K62" s="55"/>
-      <c r="L62" s="55"/>
-      <c r="M62" s="55"/>
+      <c r="H62" s="82"/>
+      <c r="I62" s="82"/>
+      <c r="J62" s="82"/>
+      <c r="K62" s="82"/>
+      <c r="L62" s="82"/>
+      <c r="M62" s="82"/>
     </row>
     <row r="63" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="55" t="s">
+      <c r="A63" s="82" t="s">
         <v>36</v>
       </c>
-      <c r="B63" s="55"/>
-      <c r="C63" s="55"/>
-      <c r="D63" s="55"/>
-      <c r="E63" s="55"/>
-      <c r="F63" s="55"/>
-      <c r="G63" s="55" t="s">
+      <c r="B63" s="82"/>
+      <c r="C63" s="82"/>
+      <c r="D63" s="82"/>
+      <c r="E63" s="82"/>
+      <c r="F63" s="82"/>
+      <c r="G63" s="82" t="s">
         <v>36</v>
       </c>
-      <c r="H63" s="55"/>
-      <c r="I63" s="55"/>
-      <c r="J63" s="55"/>
-      <c r="K63" s="55"/>
-      <c r="L63" s="55"/>
-      <c r="M63" s="55"/>
+      <c r="H63" s="82"/>
+      <c r="I63" s="82"/>
+      <c r="J63" s="82"/>
+      <c r="K63" s="82"/>
+      <c r="L63" s="82"/>
+      <c r="M63" s="82"/>
     </row>
     <row r="64" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="55" t="s">
+      <c r="A64" s="82" t="s">
         <v>35</v>
       </c>
-      <c r="B64" s="55"/>
-      <c r="C64" s="55"/>
-      <c r="D64" s="55"/>
-      <c r="E64" s="55"/>
-      <c r="F64" s="55"/>
-      <c r="G64" s="55" t="s">
+      <c r="B64" s="82"/>
+      <c r="C64" s="82"/>
+      <c r="D64" s="82"/>
+      <c r="E64" s="82"/>
+      <c r="F64" s="82"/>
+      <c r="G64" s="82" t="s">
         <v>35</v>
       </c>
-      <c r="H64" s="55"/>
-      <c r="I64" s="55"/>
-      <c r="J64" s="55"/>
-      <c r="K64" s="55"/>
-      <c r="L64" s="55"/>
-      <c r="M64" s="55"/>
+      <c r="H64" s="82"/>
+      <c r="I64" s="82"/>
+      <c r="J64" s="82"/>
+      <c r="K64" s="82"/>
+      <c r="L64" s="82"/>
+      <c r="M64" s="82"/>
     </row>
     <row r="65" spans="1:13" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="27"/>
@@ -2940,14 +3111,14 @@
       <c r="L65" s="1"/>
     </row>
     <row r="66" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="56" t="s">
+      <c r="A66" s="81" t="s">
         <v>34</v>
       </c>
-      <c r="B66" s="56"/>
-      <c r="C66" s="56"/>
-      <c r="D66" s="56"/>
-      <c r="E66" s="56"/>
-      <c r="F66" s="56"/>
+      <c r="B66" s="81"/>
+      <c r="C66" s="81"/>
+      <c r="D66" s="81"/>
+      <c r="E66" s="81"/>
+      <c r="F66" s="81"/>
     </row>
     <row r="67" spans="1:13" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="10" t="s">
@@ -3174,14 +3345,14 @@
       </c>
     </row>
     <row r="72" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="56" t="s">
+      <c r="A72" s="81" t="s">
         <v>24</v>
       </c>
-      <c r="B72" s="56"/>
-      <c r="C72" s="56"/>
-      <c r="D72" s="56"/>
-      <c r="E72" s="56"/>
-      <c r="F72" s="56"/>
+      <c r="B72" s="81"/>
+      <c r="C72" s="81"/>
+      <c r="D72" s="81"/>
+      <c r="E72" s="81"/>
+      <c r="F72" s="81"/>
     </row>
     <row r="73" spans="1:13" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="10" t="s">
@@ -3290,14 +3461,14 @@
       <c r="G77" s="5"/>
     </row>
     <row r="78" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="56" t="s">
+      <c r="A78" s="81" t="s">
         <v>23</v>
       </c>
-      <c r="B78" s="56"/>
-      <c r="C78" s="56"/>
-      <c r="D78" s="56"/>
-      <c r="E78" s="56"/>
-      <c r="F78" s="56"/>
+      <c r="B78" s="81"/>
+      <c r="C78" s="81"/>
+      <c r="D78" s="81"/>
+      <c r="E78" s="81"/>
+      <c r="F78" s="81"/>
     </row>
     <row r="79" spans="1:13" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="10" t="s">
@@ -3413,22 +3584,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A78:F78"/>
-    <mergeCell ref="A72:F72"/>
-    <mergeCell ref="A66:F66"/>
-    <mergeCell ref="G64:M64"/>
-    <mergeCell ref="G63:M63"/>
-    <mergeCell ref="G62:M62"/>
-    <mergeCell ref="A64:F64"/>
-    <mergeCell ref="A62:F62"/>
-    <mergeCell ref="A63:F63"/>
-    <mergeCell ref="A6:F6"/>
     <mergeCell ref="G1:L1"/>
     <mergeCell ref="G2:L2"/>
     <mergeCell ref="G3:L3"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A3:F3"/>
+    <mergeCell ref="G62:M62"/>
+    <mergeCell ref="A64:F64"/>
+    <mergeCell ref="A62:F62"/>
+    <mergeCell ref="A63:F63"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="A78:F78"/>
+    <mergeCell ref="A72:F72"/>
+    <mergeCell ref="A66:F66"/>
+    <mergeCell ref="G64:M64"/>
+    <mergeCell ref="G63:M63"/>
   </mergeCells>
   <pageMargins left="0.56000000000000005" right="0.3" top="0.57999999999999996" bottom="0.53" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -3439,8 +3610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG20"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -3452,86 +3623,86 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" s="39" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="57" t="s">
-        <v>90</v>
-      </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
-      <c r="I1" s="57"/>
-      <c r="J1" s="57"/>
-      <c r="K1" s="57"/>
-      <c r="L1" s="57"/>
-      <c r="M1" s="57"/>
-      <c r="N1" s="57"/>
-      <c r="O1" s="57"/>
-      <c r="P1" s="57"/>
-      <c r="Q1" s="57"/>
-      <c r="R1" s="57"/>
-      <c r="S1" s="57"/>
-      <c r="T1" s="57"/>
-      <c r="U1" s="57"/>
-      <c r="V1" s="57"/>
-      <c r="W1" s="57"/>
-      <c r="X1" s="57"/>
-      <c r="Y1" s="57"/>
-      <c r="Z1" s="57"/>
-      <c r="AA1" s="57"/>
-      <c r="AB1" s="57"/>
-      <c r="AC1" s="57"/>
-      <c r="AD1" s="57"/>
-      <c r="AE1" s="57"/>
-      <c r="AF1" s="57"/>
-      <c r="AG1" s="57"/>
+      <c r="A1" s="83" t="s">
+        <v>151</v>
+      </c>
+      <c r="B1" s="83"/>
+      <c r="C1" s="83"/>
+      <c r="D1" s="83"/>
+      <c r="E1" s="83"/>
+      <c r="F1" s="83"/>
+      <c r="G1" s="83"/>
+      <c r="H1" s="83"/>
+      <c r="I1" s="83"/>
+      <c r="J1" s="83"/>
+      <c r="K1" s="83"/>
+      <c r="L1" s="83"/>
+      <c r="M1" s="83"/>
+      <c r="N1" s="83"/>
+      <c r="O1" s="83"/>
+      <c r="P1" s="83"/>
+      <c r="Q1" s="83"/>
+      <c r="R1" s="83"/>
+      <c r="S1" s="83"/>
+      <c r="T1" s="83"/>
+      <c r="U1" s="83"/>
+      <c r="V1" s="83"/>
+      <c r="W1" s="83"/>
+      <c r="X1" s="83"/>
+      <c r="Y1" s="83"/>
+      <c r="Z1" s="83"/>
+      <c r="AA1" s="83"/>
+      <c r="AB1" s="83"/>
+      <c r="AC1" s="83"/>
+      <c r="AD1" s="83"/>
+      <c r="AE1" s="83"/>
+      <c r="AF1" s="83"/>
+      <c r="AG1" s="83"/>
     </row>
     <row r="3" spans="1:33" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="58" t="s">
+      <c r="A3" s="84" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" s="85" t="s">
         <v>68</v>
       </c>
-      <c r="B3" s="59" t="s">
+      <c r="C3" s="86" t="s">
         <v>69</v>
       </c>
-      <c r="C3" s="60" t="s">
-        <v>70</v>
-      </c>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="60"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="60"/>
-      <c r="I3" s="60"/>
-      <c r="J3" s="60"/>
-      <c r="K3" s="60"/>
-      <c r="L3" s="60"/>
-      <c r="M3" s="60"/>
-      <c r="N3" s="60"/>
-      <c r="O3" s="60"/>
-      <c r="P3" s="60"/>
-      <c r="Q3" s="60"/>
-      <c r="R3" s="60"/>
-      <c r="S3" s="60"/>
-      <c r="T3" s="60"/>
-      <c r="U3" s="60"/>
-      <c r="V3" s="60"/>
-      <c r="W3" s="60"/>
-      <c r="X3" s="60"/>
-      <c r="Y3" s="60"/>
-      <c r="Z3" s="60"/>
-      <c r="AA3" s="60"/>
-      <c r="AB3" s="60"/>
-      <c r="AC3" s="60"/>
-      <c r="AD3" s="60"/>
-      <c r="AE3" s="60"/>
-      <c r="AF3" s="60"/>
-      <c r="AG3" s="60"/>
+      <c r="D3" s="86"/>
+      <c r="E3" s="86"/>
+      <c r="F3" s="86"/>
+      <c r="G3" s="86"/>
+      <c r="H3" s="86"/>
+      <c r="I3" s="86"/>
+      <c r="J3" s="86"/>
+      <c r="K3" s="86"/>
+      <c r="L3" s="86"/>
+      <c r="M3" s="86"/>
+      <c r="N3" s="86"/>
+      <c r="O3" s="86"/>
+      <c r="P3" s="86"/>
+      <c r="Q3" s="86"/>
+      <c r="R3" s="86"/>
+      <c r="S3" s="86"/>
+      <c r="T3" s="86"/>
+      <c r="U3" s="86"/>
+      <c r="V3" s="86"/>
+      <c r="W3" s="86"/>
+      <c r="X3" s="86"/>
+      <c r="Y3" s="86"/>
+      <c r="Z3" s="86"/>
+      <c r="AA3" s="86"/>
+      <c r="AB3" s="86"/>
+      <c r="AC3" s="86"/>
+      <c r="AD3" s="86"/>
+      <c r="AE3" s="86"/>
+      <c r="AF3" s="86"/>
+      <c r="AG3" s="86"/>
     </row>
     <row r="4" spans="1:33" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="58"/>
-      <c r="B4" s="59"/>
+      <c r="A4" s="84"/>
+      <c r="B4" s="85"/>
       <c r="C4" s="41">
         <v>1</v>
       </c>
@@ -3615,8 +3786,8 @@
       </c>
     </row>
     <row r="5" spans="1:33" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="58"/>
-      <c r="B5" s="59"/>
+      <c r="A5" s="84"/>
+      <c r="B5" s="85"/>
       <c r="C5" s="42">
         <v>20</v>
       </c>
@@ -3712,100 +3883,100 @@
       </c>
     </row>
     <row r="6" spans="1:33" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="58"/>
-      <c r="B6" s="59"/>
+      <c r="A6" s="84"/>
+      <c r="B6" s="85"/>
       <c r="C6" s="44" t="s">
+        <v>70</v>
+      </c>
+      <c r="D6" s="44" t="s">
         <v>71</v>
       </c>
-      <c r="D6" s="44" t="s">
+      <c r="E6" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="E6" s="44" t="s">
+      <c r="F6" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="F6" s="44" t="s">
+      <c r="G6" s="44" t="s">
         <v>74</v>
       </c>
-      <c r="G6" s="44" t="s">
+      <c r="H6" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="H6" s="44" t="s">
+      <c r="I6" s="45" t="s">
         <v>76</v>
       </c>
-      <c r="I6" s="45" t="s">
-        <v>77</v>
-      </c>
       <c r="J6" s="44" t="s">
+        <v>70</v>
+      </c>
+      <c r="K6" s="44" t="s">
         <v>71</v>
       </c>
-      <c r="K6" s="44" t="s">
+      <c r="L6" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="L6" s="44" t="s">
+      <c r="M6" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="M6" s="44" t="s">
+      <c r="N6" s="44" t="s">
         <v>74</v>
       </c>
-      <c r="N6" s="44" t="s">
+      <c r="O6" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="O6" s="44" t="s">
+      <c r="P6" s="45" t="s">
         <v>76</v>
       </c>
-      <c r="P6" s="45" t="s">
-        <v>77</v>
-      </c>
       <c r="Q6" s="44" t="s">
+        <v>70</v>
+      </c>
+      <c r="R6" s="44" t="s">
         <v>71</v>
       </c>
-      <c r="R6" s="44" t="s">
+      <c r="S6" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="S6" s="44" t="s">
+      <c r="T6" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="T6" s="44" t="s">
+      <c r="U6" s="44" t="s">
         <v>74</v>
       </c>
-      <c r="U6" s="44" t="s">
+      <c r="V6" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="V6" s="45" t="s">
+      <c r="W6" s="45" t="s">
         <v>76</v>
       </c>
-      <c r="W6" s="45" t="s">
-        <v>77</v>
-      </c>
       <c r="X6" s="45" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y6" s="44" t="s">
         <v>71</v>
       </c>
-      <c r="Y6" s="44" t="s">
+      <c r="Z6" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="Z6" s="44" t="s">
+      <c r="AA6" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="AA6" s="44" t="s">
+      <c r="AB6" s="44" t="s">
         <v>74</v>
       </c>
-      <c r="AB6" s="44" t="s">
+      <c r="AC6" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="AC6" s="44" t="s">
+      <c r="AD6" s="45" t="s">
         <v>76</v>
       </c>
-      <c r="AD6" s="45" t="s">
-        <v>77</v>
-      </c>
       <c r="AE6" s="44" t="s">
+        <v>70</v>
+      </c>
+      <c r="AF6" s="44" t="s">
         <v>71</v>
       </c>
-      <c r="AF6" s="44" t="s">
+      <c r="AG6" s="44" t="s">
         <v>72</v>
-      </c>
-      <c r="AG6" s="44" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:33" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3907,7 +4078,7 @@
     </row>
     <row r="8" spans="1:33" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="48" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B8" s="49">
         <v>10</v>
@@ -3946,7 +4117,7 @@
     </row>
     <row r="9" spans="1:33" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="48" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B9" s="49">
         <v>20</v>
@@ -3985,7 +4156,7 @@
     </row>
     <row r="10" spans="1:33" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="48" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B10" s="49">
         <v>25</v>
@@ -4024,7 +4195,7 @@
     </row>
     <row r="11" spans="1:33" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="48" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B11" s="49">
         <v>25</v>
@@ -4063,7 +4234,7 @@
     </row>
     <row r="12" spans="1:33" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="48" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B12" s="49">
         <v>25</v>
@@ -4102,7 +4273,7 @@
     </row>
     <row r="13" spans="1:33" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="48" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B13" s="49">
         <v>14</v>
@@ -4141,7 +4312,7 @@
     </row>
     <row r="14" spans="1:33" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="48" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B14" s="49">
         <v>30</v>
@@ -4180,7 +4351,7 @@
     </row>
     <row r="15" spans="1:33" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="48" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B15" s="49">
         <v>12</v>
@@ -4219,7 +4390,7 @@
     </row>
     <row r="16" spans="1:33" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="48" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B16" s="49">
         <v>20</v>
@@ -4258,7 +4429,7 @@
     </row>
     <row r="17" spans="1:33" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="48" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B17" s="49">
         <v>10</v>
@@ -4297,7 +4468,7 @@
     </row>
     <row r="18" spans="1:33" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="48" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B18" s="49">
         <v>10</v>
@@ -4336,7 +4507,7 @@
     </row>
     <row r="19" spans="1:33" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="48" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B19" s="49">
         <v>10</v>
@@ -4381,37 +4552,37 @@
         <f>SUM(B8:B18)</f>
         <v>201</v>
       </c>
-      <c r="C20" s="61"/>
-      <c r="D20" s="62"/>
-      <c r="E20" s="62"/>
-      <c r="F20" s="62"/>
-      <c r="G20" s="62"/>
-      <c r="H20" s="62"/>
-      <c r="I20" s="62"/>
-      <c r="J20" s="62"/>
-      <c r="K20" s="62"/>
-      <c r="L20" s="62"/>
-      <c r="M20" s="62"/>
-      <c r="N20" s="62"/>
-      <c r="O20" s="62"/>
-      <c r="P20" s="62"/>
-      <c r="Q20" s="62"/>
-      <c r="R20" s="62"/>
-      <c r="S20" s="62"/>
-      <c r="T20" s="62"/>
-      <c r="U20" s="62"/>
-      <c r="V20" s="62"/>
-      <c r="W20" s="62"/>
-      <c r="X20" s="62"/>
-      <c r="Y20" s="62"/>
-      <c r="Z20" s="62"/>
-      <c r="AA20" s="62"/>
-      <c r="AB20" s="62"/>
-      <c r="AC20" s="62"/>
-      <c r="AD20" s="62"/>
-      <c r="AE20" s="62"/>
-      <c r="AF20" s="62"/>
-      <c r="AG20" s="62"/>
+      <c r="C20" s="87"/>
+      <c r="D20" s="88"/>
+      <c r="E20" s="88"/>
+      <c r="F20" s="88"/>
+      <c r="G20" s="88"/>
+      <c r="H20" s="88"/>
+      <c r="I20" s="88"/>
+      <c r="J20" s="88"/>
+      <c r="K20" s="88"/>
+      <c r="L20" s="88"/>
+      <c r="M20" s="88"/>
+      <c r="N20" s="88"/>
+      <c r="O20" s="88"/>
+      <c r="P20" s="88"/>
+      <c r="Q20" s="88"/>
+      <c r="R20" s="88"/>
+      <c r="S20" s="88"/>
+      <c r="T20" s="88"/>
+      <c r="U20" s="88"/>
+      <c r="V20" s="88"/>
+      <c r="W20" s="88"/>
+      <c r="X20" s="88"/>
+      <c r="Y20" s="88"/>
+      <c r="Z20" s="88"/>
+      <c r="AA20" s="88"/>
+      <c r="AB20" s="88"/>
+      <c r="AC20" s="88"/>
+      <c r="AD20" s="88"/>
+      <c r="AE20" s="88"/>
+      <c r="AF20" s="88"/>
+      <c r="AG20" s="88"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -4428,957 +4599,570 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:L12"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20:B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" customWidth="1"/>
-    <col min="3" max="6" width="12" customWidth="1"/>
-    <col min="7" max="7" width="4.7109375" customWidth="1"/>
-    <col min="8" max="8" width="13" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="38" t="s">
-        <v>93</v>
-      </c>
-      <c r="C3" s="38" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="38" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" s="38" t="s">
-        <v>59</v>
-      </c>
-      <c r="F3" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="53" t="s">
-        <v>93</v>
-      </c>
-      <c r="I3" s="53" t="s">
-        <v>94</v>
-      </c>
-      <c r="J3" s="53" t="s">
-        <v>95</v>
-      </c>
-      <c r="K3" s="53" t="s">
-        <v>96</v>
-      </c>
-      <c r="L3" s="53" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="38">
-        <v>1</v>
-      </c>
-      <c r="B4" s="38" t="s">
-        <v>60</v>
-      </c>
-      <c r="C4" s="38">
-        <v>25</v>
-      </c>
-      <c r="D4" s="38" t="s">
-        <v>91</v>
-      </c>
-      <c r="E4" s="38">
-        <f>VLOOKUP(B4,$H$4:$L$11,4)</f>
-        <v>7000</v>
-      </c>
-      <c r="F4" s="38">
-        <f>E4*C4</f>
-        <v>175000</v>
-      </c>
-      <c r="H4" s="38" t="s">
-        <v>60</v>
-      </c>
-      <c r="I4" s="54">
-        <v>5000</v>
-      </c>
-      <c r="J4" s="54">
-        <f>I4+1000</f>
-        <v>6000</v>
-      </c>
-      <c r="K4" s="54">
-        <f t="shared" ref="K4:L4" si="0">J4+1000</f>
-        <v>7000</v>
-      </c>
-      <c r="L4" s="54">
-        <f t="shared" si="0"/>
-        <v>8000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="38">
-        <v>2</v>
-      </c>
-      <c r="B5" s="38" t="s">
-        <v>61</v>
-      </c>
-      <c r="C5" s="38">
-        <v>25</v>
-      </c>
-      <c r="D5" s="38" t="s">
-        <v>91</v>
-      </c>
-      <c r="E5" s="38">
-        <f t="shared" ref="E5:E11" si="1">VLOOKUP(B5,$H$4:$L$11,4)</f>
-        <v>7000</v>
-      </c>
-      <c r="F5" s="38">
-        <f t="shared" ref="F5:F11" si="2">E5*C5</f>
-        <v>175000</v>
-      </c>
-      <c r="H5" s="38" t="s">
-        <v>61</v>
-      </c>
-      <c r="I5" s="54">
-        <v>5000</v>
-      </c>
-      <c r="J5" s="54">
-        <f t="shared" ref="J5:L11" si="3">I5+1000</f>
-        <v>6000</v>
-      </c>
-      <c r="K5" s="54">
-        <f t="shared" si="3"/>
-        <v>7000</v>
-      </c>
-      <c r="L5" s="54">
-        <f t="shared" si="3"/>
-        <v>8000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="38">
-        <v>3</v>
-      </c>
-      <c r="B6" s="38" t="s">
-        <v>62</v>
-      </c>
-      <c r="C6" s="38">
-        <v>25</v>
-      </c>
-      <c r="D6" s="38" t="s">
-        <v>91</v>
-      </c>
-      <c r="E6" s="38">
-        <f t="shared" si="1"/>
-        <v>7000</v>
-      </c>
-      <c r="F6" s="38">
-        <f t="shared" si="2"/>
-        <v>175000</v>
-      </c>
-      <c r="H6" s="38" t="s">
-        <v>62</v>
-      </c>
-      <c r="I6" s="54">
-        <v>13000</v>
-      </c>
-      <c r="J6" s="54">
-        <f t="shared" si="3"/>
-        <v>14000</v>
-      </c>
-      <c r="K6" s="54">
-        <f t="shared" si="3"/>
-        <v>15000</v>
-      </c>
-      <c r="L6" s="54">
-        <f t="shared" si="3"/>
-        <v>16000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="38">
-        <v>4</v>
-      </c>
-      <c r="B7" s="38" t="s">
-        <v>63</v>
-      </c>
-      <c r="C7" s="38">
-        <v>13</v>
-      </c>
-      <c r="D7" s="38" t="s">
-        <v>92</v>
-      </c>
-      <c r="E7" s="38">
-        <f t="shared" si="1"/>
-        <v>17000</v>
-      </c>
-      <c r="F7" s="38">
-        <f t="shared" si="2"/>
-        <v>221000</v>
-      </c>
-      <c r="H7" s="38" t="s">
-        <v>63</v>
-      </c>
-      <c r="I7" s="54">
-        <v>15000</v>
-      </c>
-      <c r="J7" s="54">
-        <f t="shared" si="3"/>
-        <v>16000</v>
-      </c>
-      <c r="K7" s="54">
-        <f t="shared" si="3"/>
-        <v>17000</v>
-      </c>
-      <c r="L7" s="54">
-        <f t="shared" si="3"/>
-        <v>18000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="38">
-        <v>5</v>
-      </c>
-      <c r="B8" s="38" t="s">
-        <v>64</v>
-      </c>
-      <c r="C8" s="38">
-        <v>3</v>
-      </c>
-      <c r="D8" s="38" t="s">
-        <v>3</v>
-      </c>
-      <c r="E8" s="38" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F8" s="38" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="H8" s="38" t="s">
-        <v>64</v>
-      </c>
-      <c r="I8" s="54">
-        <v>5000</v>
-      </c>
-      <c r="J8" s="54">
-        <f t="shared" si="3"/>
-        <v>6000</v>
-      </c>
-      <c r="K8" s="54">
-        <f t="shared" si="3"/>
-        <v>7000</v>
-      </c>
-      <c r="L8" s="54">
-        <f t="shared" si="3"/>
-        <v>8000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="38">
-        <v>6</v>
-      </c>
-      <c r="B9" s="38" t="s">
-        <v>65</v>
-      </c>
-      <c r="C9" s="38">
-        <v>8</v>
-      </c>
-      <c r="D9" s="38" t="s">
-        <v>3</v>
-      </c>
-      <c r="E9" s="38">
-        <f t="shared" si="1"/>
-        <v>12000</v>
-      </c>
-      <c r="F9" s="38">
-        <f t="shared" si="2"/>
-        <v>96000</v>
-      </c>
-      <c r="H9" s="38" t="s">
-        <v>65</v>
-      </c>
-      <c r="I9" s="54">
-        <v>10000</v>
-      </c>
-      <c r="J9" s="54">
-        <f t="shared" si="3"/>
-        <v>11000</v>
-      </c>
-      <c r="K9" s="54">
-        <f t="shared" si="3"/>
-        <v>12000</v>
-      </c>
-      <c r="L9" s="54">
-        <f t="shared" si="3"/>
-        <v>13000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="38">
-        <v>7</v>
-      </c>
-      <c r="B10" s="38" t="s">
-        <v>66</v>
-      </c>
-      <c r="C10" s="38">
-        <v>25</v>
-      </c>
-      <c r="D10" s="38" t="s">
-        <v>3</v>
-      </c>
-      <c r="E10" s="38">
-        <f t="shared" si="1"/>
-        <v>42000</v>
-      </c>
-      <c r="F10" s="38">
-        <f t="shared" si="2"/>
-        <v>1050000</v>
-      </c>
-      <c r="H10" s="38" t="s">
-        <v>66</v>
-      </c>
-      <c r="I10" s="54">
-        <v>40000</v>
-      </c>
-      <c r="J10" s="54">
-        <f t="shared" si="3"/>
-        <v>41000</v>
-      </c>
-      <c r="K10" s="54">
-        <f t="shared" si="3"/>
-        <v>42000</v>
-      </c>
-      <c r="L10" s="54">
-        <f t="shared" si="3"/>
-        <v>43000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="38">
-        <v>8</v>
-      </c>
-      <c r="B11" s="38" t="s">
-        <v>67</v>
-      </c>
-      <c r="C11" s="38">
-        <v>1</v>
-      </c>
-      <c r="D11" s="38" t="s">
-        <v>91</v>
-      </c>
-      <c r="E11" s="38">
-        <f t="shared" si="1"/>
-        <v>7000</v>
-      </c>
-      <c r="F11" s="38">
-        <f t="shared" si="2"/>
-        <v>7000</v>
-      </c>
-      <c r="H11" s="38" t="s">
-        <v>67</v>
-      </c>
-      <c r="I11" s="54">
-        <v>200000</v>
-      </c>
-      <c r="J11" s="54">
-        <f t="shared" si="3"/>
-        <v>201000</v>
-      </c>
-      <c r="K11" s="54">
-        <f t="shared" si="3"/>
-        <v>202000</v>
-      </c>
-      <c r="L11" s="54">
-        <f t="shared" si="3"/>
-        <v>203000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="38"/>
-      <c r="B12" s="38"/>
-      <c r="C12" s="38"/>
-      <c r="D12" s="38"/>
-      <c r="E12" s="38"/>
-      <c r="F12" s="38"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H30"/>
-  <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="5.28515625" style="86" customWidth="1"/>
-    <col min="2" max="2" width="26.85546875" style="64" customWidth="1"/>
-    <col min="3" max="3" width="33.42578125" style="64" customWidth="1"/>
-    <col min="4" max="4" width="26.140625" style="64" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" style="64" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" style="64" customWidth="1"/>
-    <col min="7" max="8" width="15.140625" style="64" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="64"/>
+    <col min="1" max="1" width="5.28515625" style="72" customWidth="1"/>
+    <col min="2" max="2" width="26.85546875" style="55" customWidth="1"/>
+    <col min="3" max="3" width="33.42578125" style="55" customWidth="1"/>
+    <col min="4" max="4" width="26.140625" style="55" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" style="55" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" style="55" customWidth="1"/>
+    <col min="7" max="8" width="15.140625" style="55" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="55"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="89" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" s="89"/>
+      <c r="C1" s="89"/>
+      <c r="D1" s="89"/>
+      <c r="E1" s="89"/>
+      <c r="F1" s="89"/>
+      <c r="G1" s="89"/>
+      <c r="H1" s="89"/>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="89" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" s="89"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="89"/>
+      <c r="E2" s="89"/>
+      <c r="F2" s="89"/>
+      <c r="G2" s="89"/>
+      <c r="H2" s="89"/>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="56"/>
+      <c r="B3" s="56"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
+      <c r="E3" s="56"/>
+      <c r="F3" s="56"/>
+      <c r="G3" s="56"/>
+      <c r="H3" s="56"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="57"/>
+    </row>
+    <row r="5" spans="1:8" s="61" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="58" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="59" t="s">
         <v>98</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-    </row>
-    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="63" t="s">
+      <c r="C5" s="59" t="s">
         <v>99</v>
       </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="63"/>
-      <c r="H2" s="63"/>
-    </row>
-    <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="65"/>
-      <c r="B3" s="65"/>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="65"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="66"/>
-    </row>
-    <row r="5" spans="1:8" s="70" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="67" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="68" t="s">
+      <c r="D5" s="59" t="s">
         <v>100</v>
       </c>
-      <c r="C5" s="68" t="s">
+      <c r="E5" s="60" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="59" t="s">
+        <v>0</v>
+      </c>
+      <c r="G5" s="60" t="s">
         <v>101</v>
       </c>
-      <c r="D5" s="68" t="s">
+      <c r="H5" s="60" t="s">
         <v>102</v>
       </c>
-      <c r="E5" s="69" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="68" t="s">
-        <v>0</v>
-      </c>
-      <c r="G5" s="69" t="s">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="90"/>
+      <c r="B6" s="91"/>
+      <c r="C6" s="91"/>
+      <c r="D6" s="91"/>
+      <c r="E6" s="91"/>
+      <c r="F6" s="91"/>
+      <c r="G6" s="91"/>
+      <c r="H6" s="92"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="62">
+        <v>1</v>
+      </c>
+      <c r="B7" s="63" t="s">
         <v>103</v>
       </c>
-      <c r="H5" s="69" t="s">
+      <c r="C7" s="63" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="71"/>
-      <c r="B6" s="72"/>
-      <c r="C6" s="72"/>
-      <c r="D6" s="72"/>
-      <c r="E6" s="72"/>
-      <c r="F6" s="72"/>
-      <c r="G6" s="72"/>
-      <c r="H6" s="73"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="74">
+      <c r="D7" s="63" t="s">
+        <v>105</v>
+      </c>
+      <c r="E7" s="64">
         <v>1</v>
       </c>
-      <c r="B7" s="75" t="s">
-        <v>105</v>
-      </c>
-      <c r="C7" s="75" t="s">
+      <c r="F7" s="63" t="s">
         <v>106</v>
       </c>
-      <c r="D7" s="75" t="s">
-        <v>107</v>
-      </c>
-      <c r="E7" s="76">
-        <v>1</v>
-      </c>
-      <c r="F7" s="75" t="s">
-        <v>108</v>
-      </c>
-      <c r="G7" s="77">
+      <c r="G7" s="65">
         <v>480000</v>
       </c>
-      <c r="H7" s="77">
+      <c r="H7" s="65">
         <f t="shared" ref="H7:H21" si="0">G7*E7</f>
         <v>480000</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="74">
+      <c r="A8" s="62">
         <v>2</v>
       </c>
-      <c r="B8" s="75" t="s">
+      <c r="B8" s="63" t="s">
+        <v>107</v>
+      </c>
+      <c r="C8" s="63" t="s">
+        <v>108</v>
+      </c>
+      <c r="D8" s="63" t="s">
+        <v>105</v>
+      </c>
+      <c r="E8" s="64">
+        <v>4</v>
+      </c>
+      <c r="F8" s="63" t="s">
         <v>109</v>
       </c>
-      <c r="C8" s="75" t="s">
-        <v>110</v>
-      </c>
-      <c r="D8" s="75" t="s">
-        <v>107</v>
-      </c>
-      <c r="E8" s="76">
-        <v>4</v>
-      </c>
-      <c r="F8" s="75" t="s">
-        <v>111</v>
-      </c>
-      <c r="G8" s="77">
+      <c r="G8" s="65">
         <v>45000</v>
       </c>
-      <c r="H8" s="77">
+      <c r="H8" s="65">
         <f t="shared" si="0"/>
         <v>180000</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="74">
+      <c r="A9" s="62">
         <v>3</v>
       </c>
-      <c r="B9" s="75" t="s">
+      <c r="B9" s="63" t="s">
+        <v>110</v>
+      </c>
+      <c r="C9" s="63" t="s">
+        <v>111</v>
+      </c>
+      <c r="D9" s="63" t="s">
         <v>112</v>
       </c>
-      <c r="C9" s="75" t="s">
-        <v>113</v>
-      </c>
-      <c r="D9" s="75" t="s">
-        <v>114</v>
-      </c>
-      <c r="E9" s="76">
+      <c r="E9" s="64">
         <v>7</v>
       </c>
-      <c r="F9" s="75" t="s">
+      <c r="F9" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="G9" s="77">
+      <c r="G9" s="65">
         <v>10000</v>
       </c>
-      <c r="H9" s="77">
+      <c r="H9" s="65">
         <f t="shared" si="0"/>
         <v>70000</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="74">
+      <c r="A10" s="62">
         <v>4</v>
       </c>
-      <c r="B10" s="75" t="s">
+      <c r="B10" s="63" t="s">
+        <v>113</v>
+      </c>
+      <c r="C10" s="63" t="s">
+        <v>114</v>
+      </c>
+      <c r="D10" s="63" t="s">
         <v>115</v>
       </c>
-      <c r="C10" s="75" t="s">
-        <v>116</v>
-      </c>
-      <c r="D10" s="75" t="s">
-        <v>117</v>
-      </c>
-      <c r="E10" s="76">
+      <c r="E10" s="64">
         <v>6</v>
       </c>
-      <c r="F10" s="75" t="s">
+      <c r="F10" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="G10" s="77">
+      <c r="G10" s="65">
         <v>180000</v>
       </c>
-      <c r="H10" s="77">
+      <c r="H10" s="65">
         <f>G10*E10</f>
         <v>1080000</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="74">
+      <c r="A11" s="62">
         <v>5</v>
       </c>
-      <c r="B11" s="75" t="s">
+      <c r="B11" s="63" t="s">
+        <v>116</v>
+      </c>
+      <c r="C11" s="63" t="s">
+        <v>117</v>
+      </c>
+      <c r="D11" s="63" t="s">
         <v>118</v>
       </c>
-      <c r="C11" s="75" t="s">
-        <v>119</v>
-      </c>
-      <c r="D11" s="75" t="s">
-        <v>120</v>
-      </c>
-      <c r="E11" s="76">
+      <c r="E11" s="64">
         <v>6</v>
       </c>
-      <c r="F11" s="75" t="s">
+      <c r="F11" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="G11" s="77">
+      <c r="G11" s="65">
         <v>45000</v>
       </c>
-      <c r="H11" s="77">
+      <c r="H11" s="65">
         <f>G11*E11</f>
         <v>270000</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="74">
+      <c r="A12" s="62">
         <v>6</v>
       </c>
-      <c r="B12" s="64" t="s">
+      <c r="B12" s="55" t="s">
+        <v>119</v>
+      </c>
+      <c r="C12" s="63" t="s">
+        <v>120</v>
+      </c>
+      <c r="D12" s="63" t="s">
         <v>121</v>
       </c>
-      <c r="C12" s="75" t="s">
-        <v>122</v>
-      </c>
-      <c r="D12" s="75" t="s">
-        <v>123</v>
-      </c>
-      <c r="E12" s="76">
+      <c r="E12" s="64">
         <v>6</v>
       </c>
-      <c r="F12" s="75" t="s">
+      <c r="F12" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="G12" s="77">
+      <c r="G12" s="65">
         <v>100000</v>
       </c>
-      <c r="H12" s="77">
+      <c r="H12" s="65">
         <f>G12*E12</f>
         <v>600000</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="74">
+      <c r="A13" s="62">
         <v>7</v>
       </c>
-      <c r="B13" s="75" t="s">
+      <c r="B13" s="63" t="s">
+        <v>122</v>
+      </c>
+      <c r="C13" s="63" t="s">
+        <v>123</v>
+      </c>
+      <c r="D13" s="63" t="s">
         <v>124</v>
       </c>
-      <c r="C13" s="75" t="s">
-        <v>125</v>
-      </c>
-      <c r="D13" s="75" t="s">
-        <v>126</v>
-      </c>
-      <c r="E13" s="76">
+      <c r="E13" s="64">
         <v>1</v>
       </c>
-      <c r="F13" s="75" t="s">
+      <c r="F13" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="G13" s="77">
+      <c r="G13" s="65">
         <v>400000</v>
       </c>
-      <c r="H13" s="77">
+      <c r="H13" s="65">
         <f t="shared" ref="H13" si="1">G13*E13</f>
         <v>400000</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="74">
+      <c r="A14" s="62">
         <v>8</v>
       </c>
-      <c r="B14" s="75" t="s">
+      <c r="B14" s="63" t="s">
+        <v>125</v>
+      </c>
+      <c r="C14" s="63" t="s">
+        <v>126</v>
+      </c>
+      <c r="D14" s="63" t="s">
         <v>127</v>
       </c>
-      <c r="C14" s="75" t="s">
-        <v>128</v>
-      </c>
-      <c r="D14" s="75" t="s">
-        <v>129</v>
-      </c>
-      <c r="E14" s="76">
+      <c r="E14" s="64">
         <v>4</v>
       </c>
-      <c r="F14" s="75" t="s">
-        <v>111</v>
-      </c>
-      <c r="G14" s="77">
+      <c r="F14" s="63" t="s">
+        <v>109</v>
+      </c>
+      <c r="G14" s="65">
         <v>45000</v>
       </c>
-      <c r="H14" s="77">
+      <c r="H14" s="65">
         <f t="shared" si="0"/>
         <v>180000</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="74">
+      <c r="A15" s="62">
         <v>9</v>
       </c>
-      <c r="B15" s="75" t="s">
+      <c r="B15" s="63" t="s">
+        <v>128</v>
+      </c>
+      <c r="C15" s="63" t="s">
+        <v>129</v>
+      </c>
+      <c r="D15" s="63" t="s">
         <v>130</v>
       </c>
-      <c r="C15" s="75" t="s">
-        <v>131</v>
-      </c>
-      <c r="D15" s="75" t="s">
-        <v>132</v>
-      </c>
-      <c r="E15" s="76">
+      <c r="E15" s="64">
         <v>6</v>
       </c>
-      <c r="F15" s="75" t="s">
+      <c r="F15" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="G15" s="77">
+      <c r="G15" s="65">
         <v>12000</v>
       </c>
-      <c r="H15" s="77">
+      <c r="H15" s="65">
         <f t="shared" si="0"/>
         <v>72000</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="74">
+      <c r="A16" s="62">
         <v>10</v>
       </c>
-      <c r="B16" s="75" t="s">
-        <v>133</v>
-      </c>
-      <c r="C16" s="75" t="s">
-        <v>134</v>
-      </c>
-      <c r="D16" s="75" t="s">
+      <c r="B16" s="63" t="s">
+        <v>131</v>
+      </c>
+      <c r="C16" s="63" t="s">
         <v>132</v>
       </c>
-      <c r="E16" s="76">
+      <c r="D16" s="63" t="s">
+        <v>130</v>
+      </c>
+      <c r="E16" s="64">
         <v>6</v>
       </c>
-      <c r="F16" s="75" t="s">
+      <c r="F16" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="G16" s="77">
+      <c r="G16" s="65">
         <v>10000</v>
       </c>
-      <c r="H16" s="77">
+      <c r="H16" s="65">
         <f t="shared" si="0"/>
         <v>60000</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="74">
+      <c r="A17" s="62">
         <v>11</v>
       </c>
-      <c r="B17" s="75" t="s">
-        <v>135</v>
-      </c>
-      <c r="C17" s="75" t="s">
-        <v>136</v>
-      </c>
-      <c r="D17" s="75" t="s">
-        <v>132</v>
-      </c>
-      <c r="E17" s="76">
+      <c r="B17" s="63" t="s">
+        <v>133</v>
+      </c>
+      <c r="C17" s="63" t="s">
+        <v>134</v>
+      </c>
+      <c r="D17" s="63" t="s">
+        <v>130</v>
+      </c>
+      <c r="E17" s="64">
         <v>6</v>
       </c>
-      <c r="F17" s="75" t="s">
+      <c r="F17" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="G17" s="77">
+      <c r="G17" s="65">
         <v>8000</v>
       </c>
-      <c r="H17" s="77">
+      <c r="H17" s="65">
         <f t="shared" si="0"/>
         <v>48000</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="74">
+      <c r="A18" s="62">
         <v>12</v>
       </c>
-      <c r="B18" s="75" t="s">
+      <c r="B18" s="63" t="s">
+        <v>135</v>
+      </c>
+      <c r="C18" s="63" t="s">
+        <v>136</v>
+      </c>
+      <c r="D18" s="63" t="s">
         <v>137</v>
       </c>
-      <c r="C18" s="75" t="s">
-        <v>138</v>
-      </c>
-      <c r="D18" s="75" t="s">
-        <v>139</v>
-      </c>
-      <c r="E18" s="76">
+      <c r="E18" s="64">
         <v>6</v>
       </c>
-      <c r="F18" s="75" t="s">
+      <c r="F18" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="G18" s="77">
+      <c r="G18" s="65">
         <v>10000</v>
       </c>
-      <c r="H18" s="77">
+      <c r="H18" s="65">
         <f t="shared" si="0"/>
         <v>60000</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="74">
+      <c r="A19" s="62">
         <v>13</v>
       </c>
-      <c r="B19" s="75" t="s">
+      <c r="B19" s="63" t="s">
+        <v>138</v>
+      </c>
+      <c r="C19" s="63" t="s">
+        <v>139</v>
+      </c>
+      <c r="D19" s="63" t="s">
         <v>140</v>
       </c>
-      <c r="C19" s="75" t="s">
-        <v>141</v>
-      </c>
-      <c r="D19" s="75" t="s">
-        <v>142</v>
-      </c>
-      <c r="E19" s="76">
+      <c r="E19" s="64">
         <v>6</v>
       </c>
-      <c r="F19" s="75" t="s">
+      <c r="F19" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="G19" s="77">
+      <c r="G19" s="65">
         <v>80000</v>
       </c>
-      <c r="H19" s="77">
+      <c r="H19" s="65">
         <f t="shared" si="0"/>
         <v>480000</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="74">
+      <c r="A20" s="62">
         <v>14</v>
       </c>
-      <c r="B20" s="75" t="s">
+      <c r="B20" s="63" t="s">
+        <v>141</v>
+      </c>
+      <c r="C20" s="63" t="s">
+        <v>142</v>
+      </c>
+      <c r="D20" s="63" t="s">
         <v>143</v>
       </c>
-      <c r="C20" s="75" t="s">
-        <v>144</v>
-      </c>
-      <c r="D20" s="75" t="s">
-        <v>145</v>
-      </c>
-      <c r="E20" s="76">
+      <c r="E20" s="64">
         <v>6</v>
       </c>
-      <c r="F20" s="75" t="s">
+      <c r="F20" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="G20" s="77">
+      <c r="G20" s="65">
         <v>90000</v>
       </c>
-      <c r="H20" s="77">
+      <c r="H20" s="65">
         <f t="shared" si="0"/>
         <v>540000</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="74">
+      <c r="A21" s="62">
         <v>15</v>
       </c>
-      <c r="B21" s="75" t="s">
+      <c r="B21" s="63" t="s">
+        <v>144</v>
+      </c>
+      <c r="C21" s="63" t="s">
+        <v>145</v>
+      </c>
+      <c r="D21" s="63" t="s">
         <v>146</v>
       </c>
-      <c r="C21" s="75" t="s">
-        <v>147</v>
-      </c>
-      <c r="D21" s="75" t="s">
-        <v>148</v>
-      </c>
-      <c r="E21" s="76">
+      <c r="E21" s="64">
         <v>6</v>
       </c>
-      <c r="F21" s="75" t="s">
+      <c r="F21" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="G21" s="77">
+      <c r="G21" s="65">
         <v>80000</v>
       </c>
-      <c r="H21" s="77">
+      <c r="H21" s="65">
         <f t="shared" si="0"/>
         <v>480000</v>
       </c>
     </row>
-    <row r="22" spans="1:8" s="82" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="78" t="s">
+    <row r="22" spans="1:8" s="68" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="93" t="s">
         <v>8</v>
       </c>
-      <c r="B22" s="79"/>
-      <c r="C22" s="80"/>
-      <c r="D22" s="80"/>
-      <c r="E22" s="80"/>
-      <c r="F22" s="80"/>
-      <c r="G22" s="80"/>
-      <c r="H22" s="81">
+      <c r="B22" s="94"/>
+      <c r="C22" s="66"/>
+      <c r="D22" s="66"/>
+      <c r="E22" s="66"/>
+      <c r="F22" s="66"/>
+      <c r="G22" s="66"/>
+      <c r="H22" s="67">
         <f>SUM(H7:H21)</f>
         <v>5000000</v>
       </c>
     </row>
-    <row r="23" spans="1:8" s="82" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="83"/>
-      <c r="B23" s="83"/>
-      <c r="C23" s="84"/>
-      <c r="D23" s="84"/>
-      <c r="E23" s="84"/>
-      <c r="F23" s="84"/>
-      <c r="G23" s="84"/>
-      <c r="H23" s="85"/>
+    <row r="23" spans="1:8" s="68" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="69"/>
+      <c r="B23" s="69"/>
+      <c r="C23" s="70"/>
+      <c r="D23" s="70"/>
+      <c r="E23" s="70"/>
+      <c r="F23" s="70"/>
+      <c r="G23" s="70"/>
+      <c r="H23" s="71"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D25" s="87"/>
-      <c r="E25" s="88"/>
-      <c r="G25" s="86" t="s">
+      <c r="D25" s="73"/>
+      <c r="E25" s="74"/>
+      <c r="G25" s="72" t="s">
+        <v>147</v>
+      </c>
+      <c r="H25" s="75"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D26" s="76"/>
+      <c r="E26" s="76"/>
+      <c r="G26" s="77" t="s">
+        <v>148</v>
+      </c>
+      <c r="H26" s="75"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D27" s="76"/>
+      <c r="E27" s="76"/>
+      <c r="G27" s="78"/>
+      <c r="H27" s="75"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D28" s="76"/>
+      <c r="E28" s="76"/>
+      <c r="G28" s="75"/>
+      <c r="H28" s="75"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D29" s="76"/>
+      <c r="E29" s="76"/>
+      <c r="G29" s="79" t="s">
         <v>149</v>
       </c>
-      <c r="H25" s="89"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D26" s="90"/>
-      <c r="E26" s="90"/>
-      <c r="G26" s="91" t="s">
+      <c r="H29" s="75"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D30" s="76"/>
+      <c r="E30" s="76"/>
+      <c r="G30" s="80" t="s">
         <v>150</v>
       </c>
-      <c r="H26" s="89"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D27" s="90"/>
-      <c r="E27" s="90"/>
-      <c r="G27" s="92"/>
-      <c r="H27" s="89"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D28" s="90"/>
-      <c r="E28" s="90"/>
-      <c r="G28" s="89"/>
-      <c r="H28" s="89"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D29" s="90"/>
-      <c r="E29" s="90"/>
-      <c r="G29" s="93" t="s">
-        <v>151</v>
-      </c>
-      <c r="H29" s="89"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D30" s="90"/>
-      <c r="E30" s="90"/>
-      <c r="G30" s="94" t="s">
-        <v>152</v>
-      </c>
-      <c r="H30" s="89"/>
+      <c r="H30" s="75"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -5390,4 +5174,1797 @@
   <pageMargins left="0.36" right="0.35" top="0.65" bottom="0.4" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:G18"/>
+  <sheetViews>
+    <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="53" t="s">
+        <v>91</v>
+      </c>
+      <c r="C3" s="53" t="s">
+        <v>92</v>
+      </c>
+      <c r="D3" s="53" t="s">
+        <v>93</v>
+      </c>
+      <c r="E3" s="53" t="s">
+        <v>94</v>
+      </c>
+      <c r="F3" s="53" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="96">
+        <v>1</v>
+      </c>
+      <c r="B4" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" s="54">
+        <v>5000</v>
+      </c>
+      <c r="D4" s="54">
+        <f>C4+1000</f>
+        <v>6000</v>
+      </c>
+      <c r="E4" s="54">
+        <f>D4+1000</f>
+        <v>7000</v>
+      </c>
+      <c r="F4" s="54">
+        <f>E4+1000</f>
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="96">
+        <v>2</v>
+      </c>
+      <c r="B5" s="38" t="s">
+        <v>61</v>
+      </c>
+      <c r="C5" s="54">
+        <v>5000</v>
+      </c>
+      <c r="D5" s="54">
+        <f>C5+1000</f>
+        <v>6000</v>
+      </c>
+      <c r="E5" s="54">
+        <f>D5+1000</f>
+        <v>7000</v>
+      </c>
+      <c r="F5" s="54">
+        <f>E5+1000</f>
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="96">
+        <v>3</v>
+      </c>
+      <c r="B6" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" s="54">
+        <v>13000</v>
+      </c>
+      <c r="D6" s="54">
+        <f>C6+1000</f>
+        <v>14000</v>
+      </c>
+      <c r="E6" s="54">
+        <f>D6+1000</f>
+        <v>15000</v>
+      </c>
+      <c r="F6" s="54">
+        <f>E6+1000</f>
+        <v>16000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="96">
+        <v>4</v>
+      </c>
+      <c r="B7" s="38" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" s="54">
+        <v>15000</v>
+      </c>
+      <c r="D7" s="54">
+        <f>C7+1000</f>
+        <v>16000</v>
+      </c>
+      <c r="E7" s="54">
+        <f>D7+1000</f>
+        <v>17000</v>
+      </c>
+      <c r="F7" s="54">
+        <f>E7+1000</f>
+        <v>18000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="96">
+        <v>5</v>
+      </c>
+      <c r="B8" s="38" t="s">
+        <v>152</v>
+      </c>
+      <c r="C8" s="54">
+        <v>5000</v>
+      </c>
+      <c r="D8" s="54">
+        <f>C8+1000</f>
+        <v>6000</v>
+      </c>
+      <c r="E8" s="54">
+        <f>D8+1000</f>
+        <v>7000</v>
+      </c>
+      <c r="F8" s="54">
+        <f>E8+1000</f>
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="96">
+        <v>6</v>
+      </c>
+      <c r="B9" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="54">
+        <v>10000</v>
+      </c>
+      <c r="D9" s="54">
+        <f>C9+1000</f>
+        <v>11000</v>
+      </c>
+      <c r="E9" s="54">
+        <f>D9+1000</f>
+        <v>12000</v>
+      </c>
+      <c r="F9" s="54">
+        <f>E9+1000</f>
+        <v>13000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="96">
+        <v>7</v>
+      </c>
+      <c r="B10" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" s="54">
+        <v>40000</v>
+      </c>
+      <c r="D10" s="54">
+        <f>C10+1000</f>
+        <v>41000</v>
+      </c>
+      <c r="E10" s="54">
+        <f>D10+1000</f>
+        <v>42000</v>
+      </c>
+      <c r="F10" s="54">
+        <f>E10+1000</f>
+        <v>43000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="96">
+        <v>8</v>
+      </c>
+      <c r="B11" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" s="54">
+        <v>200000</v>
+      </c>
+      <c r="D11" s="54">
+        <f>C11+1000</f>
+        <v>201000</v>
+      </c>
+      <c r="E11" s="54">
+        <f>D11+1000</f>
+        <v>202000</v>
+      </c>
+      <c r="F11" s="54">
+        <f>E11+1000</f>
+        <v>203000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="104">
+        <v>9</v>
+      </c>
+      <c r="B12" s="103" t="s">
+        <v>157</v>
+      </c>
+      <c r="C12" s="105">
+        <v>100000</v>
+      </c>
+      <c r="D12" s="105">
+        <f>C12+1000</f>
+        <v>101000</v>
+      </c>
+      <c r="E12" s="105">
+        <f>D12+1000</f>
+        <v>102000</v>
+      </c>
+      <c r="F12" s="105">
+        <f>E12+1000</f>
+        <v>103000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="104">
+        <v>10</v>
+      </c>
+      <c r="B13" s="103" t="s">
+        <v>158</v>
+      </c>
+      <c r="C13" s="105">
+        <v>500000</v>
+      </c>
+      <c r="D13" s="105">
+        <f>C13+1000</f>
+        <v>501000</v>
+      </c>
+      <c r="E13" s="105">
+        <f>D13+1000</f>
+        <v>502000</v>
+      </c>
+      <c r="F13" s="105">
+        <f>E13+1000</f>
+        <v>503000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="95" t="s">
+        <v>165</v>
+      </c>
+      <c r="B16" s="38" t="s">
+        <v>159</v>
+      </c>
+      <c r="C16" s="38" t="s">
+        <v>160</v>
+      </c>
+      <c r="D16" s="38" t="s">
+        <v>161</v>
+      </c>
+      <c r="E16" s="38" t="s">
+        <v>162</v>
+      </c>
+      <c r="F16" s="38" t="s">
+        <v>163</v>
+      </c>
+      <c r="G16" s="38" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="95" t="s">
+        <v>171</v>
+      </c>
+      <c r="B17" s="38" t="s">
+        <v>166</v>
+      </c>
+      <c r="C17" s="38" t="s">
+        <v>166</v>
+      </c>
+      <c r="D17" s="38" t="s">
+        <v>167</v>
+      </c>
+      <c r="E17" s="38" t="s">
+        <v>168</v>
+      </c>
+      <c r="F17" s="38" t="s">
+        <v>169</v>
+      </c>
+      <c r="G17" s="38" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="95" t="s">
+        <v>172</v>
+      </c>
+      <c r="B18" s="38" t="s">
+        <v>173</v>
+      </c>
+      <c r="C18" s="38" t="s">
+        <v>173</v>
+      </c>
+      <c r="D18" s="38" t="s">
+        <v>174</v>
+      </c>
+      <c r="E18" s="38" t="s">
+        <v>167</v>
+      </c>
+      <c r="F18" s="38" t="s">
+        <v>175</v>
+      </c>
+      <c r="G18" s="38" t="s">
+        <v>176</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F19"/>
+  <sheetViews>
+    <sheetView view="pageBreakPreview" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" customWidth="1"/>
+    <col min="3" max="6" width="12" customWidth="1"/>
+    <col min="7" max="7" width="4.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="97" t="s">
+        <v>153</v>
+      </c>
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="97"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="95" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="95" t="s">
+        <v>91</v>
+      </c>
+      <c r="C3" s="95" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="95" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="95" t="s">
+        <v>59</v>
+      </c>
+      <c r="F3" s="95" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="38">
+        <v>1</v>
+      </c>
+      <c r="B4" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" s="38">
+        <v>25</v>
+      </c>
+      <c r="D4" s="38" t="s">
+        <v>89</v>
+      </c>
+      <c r="E4" s="54">
+        <f>VLOOKUP(B4,'daftar harga'!$B$4:$F$11,3)</f>
+        <v>6000</v>
+      </c>
+      <c r="F4" s="54">
+        <f>E4*C4</f>
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="38">
+        <v>2</v>
+      </c>
+      <c r="B5" s="38" t="s">
+        <v>61</v>
+      </c>
+      <c r="C5" s="38">
+        <v>25</v>
+      </c>
+      <c r="D5" s="38" t="s">
+        <v>89</v>
+      </c>
+      <c r="E5" s="54">
+        <f>VLOOKUP(B5,'daftar harga'!$B$4:$F$11,3)</f>
+        <v>6000</v>
+      </c>
+      <c r="F5" s="54">
+        <f>E5*C5</f>
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="38">
+        <v>3</v>
+      </c>
+      <c r="B6" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" s="38">
+        <v>25</v>
+      </c>
+      <c r="D6" s="38" t="s">
+        <v>89</v>
+      </c>
+      <c r="E6" s="54">
+        <f>VLOOKUP(B6,'daftar harga'!$B$4:$F$11,3)</f>
+        <v>6000</v>
+      </c>
+      <c r="F6" s="54">
+        <f>E6*C6</f>
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="38">
+        <v>4</v>
+      </c>
+      <c r="B7" s="38" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" s="38">
+        <v>13</v>
+      </c>
+      <c r="D7" s="38" t="s">
+        <v>90</v>
+      </c>
+      <c r="E7" s="54">
+        <f>VLOOKUP(B7,'daftar harga'!$B$4:$F$11,3)</f>
+        <v>16000</v>
+      </c>
+      <c r="F7" s="54">
+        <f>E7*C7</f>
+        <v>208000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="38">
+        <v>5</v>
+      </c>
+      <c r="B8" s="38" t="s">
+        <v>152</v>
+      </c>
+      <c r="C8" s="38">
+        <v>3</v>
+      </c>
+      <c r="D8" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="54">
+        <f>VLOOKUP(B8,'daftar harga'!$B$4:$F$11,3)</f>
+        <v>6000</v>
+      </c>
+      <c r="F8" s="54">
+        <f>E8*C8</f>
+        <v>18000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="38">
+        <v>6</v>
+      </c>
+      <c r="B9" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="38">
+        <v>8</v>
+      </c>
+      <c r="D9" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="54">
+        <f>VLOOKUP(B9,'daftar harga'!$B$4:$F$11,3)</f>
+        <v>11000</v>
+      </c>
+      <c r="F9" s="54">
+        <f>E9*C9</f>
+        <v>88000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="38">
+        <v>7</v>
+      </c>
+      <c r="B10" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" s="38">
+        <v>25</v>
+      </c>
+      <c r="D10" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="54">
+        <f>VLOOKUP(B10,'daftar harga'!$B$4:$F$11,3)</f>
+        <v>41000</v>
+      </c>
+      <c r="F10" s="54">
+        <f>E10*C10</f>
+        <v>1025000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="38">
+        <v>8</v>
+      </c>
+      <c r="B11" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" s="38">
+        <v>1</v>
+      </c>
+      <c r="D11" s="38" t="s">
+        <v>89</v>
+      </c>
+      <c r="E11" s="54">
+        <f>VLOOKUP(B11,'daftar harga'!$B$4:$F$11,3)</f>
+        <v>16000</v>
+      </c>
+      <c r="F11" s="54">
+        <f>E11*C11</f>
+        <v>16000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="38"/>
+      <c r="B12" s="38"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E18" s="98" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="19" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E19" s="99" t="s">
+        <v>156</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F18"/>
+  <sheetViews>
+    <sheetView view="pageBreakPreview" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" customWidth="1"/>
+    <col min="3" max="6" width="12" customWidth="1"/>
+    <col min="7" max="7" width="4.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="97" t="s">
+        <v>153</v>
+      </c>
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="97"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="95" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="95" t="s">
+        <v>91</v>
+      </c>
+      <c r="C3" s="95" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="95" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="95" t="s">
+        <v>59</v>
+      </c>
+      <c r="F3" s="95" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="38">
+        <v>1</v>
+      </c>
+      <c r="B4" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" s="38">
+        <v>25</v>
+      </c>
+      <c r="D4" s="38" t="s">
+        <v>89</v>
+      </c>
+      <c r="E4" s="54">
+        <f>VLOOKUP(B4,'daftar harga'!$B$4:$F$11,2)</f>
+        <v>5000</v>
+      </c>
+      <c r="F4" s="54">
+        <f>E4*C4</f>
+        <v>125000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="38">
+        <v>2</v>
+      </c>
+      <c r="B5" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="38">
+        <v>25</v>
+      </c>
+      <c r="D5" s="38" t="s">
+        <v>89</v>
+      </c>
+      <c r="E5" s="54">
+        <f>VLOOKUP(B5,'daftar harga'!$B$4:$F$11,2)</f>
+        <v>5000</v>
+      </c>
+      <c r="F5" s="54">
+        <f>E5*C5</f>
+        <v>125000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="38">
+        <v>3</v>
+      </c>
+      <c r="B6" s="38" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="38">
+        <v>13</v>
+      </c>
+      <c r="D6" s="38" t="s">
+        <v>90</v>
+      </c>
+      <c r="E6" s="54">
+        <f>VLOOKUP(B6,'daftar harga'!$B$4:$F$11,2)</f>
+        <v>15000</v>
+      </c>
+      <c r="F6" s="54">
+        <f>E6*C6</f>
+        <v>195000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="38">
+        <v>4</v>
+      </c>
+      <c r="B7" s="38" t="s">
+        <v>152</v>
+      </c>
+      <c r="C7" s="38">
+        <v>3</v>
+      </c>
+      <c r="D7" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="54">
+        <f>VLOOKUP(B7,'daftar harga'!$B$4:$F$11,2)</f>
+        <v>5000</v>
+      </c>
+      <c r="F7" s="54">
+        <f>E7*C7</f>
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="38">
+        <v>5</v>
+      </c>
+      <c r="B8" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" s="38">
+        <v>8</v>
+      </c>
+      <c r="D8" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="54">
+        <f>VLOOKUP(B8,'daftar harga'!$B$4:$F$11,2)</f>
+        <v>10000</v>
+      </c>
+      <c r="F8" s="54">
+        <f>E8*C8</f>
+        <v>80000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="38">
+        <v>6</v>
+      </c>
+      <c r="B9" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="C9" s="38">
+        <v>1</v>
+      </c>
+      <c r="D9" s="38" t="s">
+        <v>89</v>
+      </c>
+      <c r="E9" s="54">
+        <f>VLOOKUP(B9,'daftar harga'!$B$4:$F$11,2)</f>
+        <v>15000</v>
+      </c>
+      <c r="F9" s="54">
+        <f>E9*C9</f>
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="38">
+        <v>7</v>
+      </c>
+      <c r="B10" s="103" t="s">
+        <v>157</v>
+      </c>
+      <c r="C10" s="38">
+        <v>1</v>
+      </c>
+      <c r="D10" s="38" t="s">
+        <v>89</v>
+      </c>
+      <c r="E10" s="54">
+        <f>VLOOKUP(B10,'daftar harga'!$B$4:$F$11,2)</f>
+        <v>200000</v>
+      </c>
+      <c r="F10" s="54">
+        <f t="shared" ref="F10:F11" si="0">E10*C10</f>
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="38">
+        <v>8</v>
+      </c>
+      <c r="B11" s="103" t="s">
+        <v>158</v>
+      </c>
+      <c r="C11" s="38">
+        <v>1</v>
+      </c>
+      <c r="D11" s="38" t="s">
+        <v>89</v>
+      </c>
+      <c r="E11" s="54">
+        <f>VLOOKUP(B11,'daftar harga'!$B$4:$F$11,2)</f>
+        <v>5000</v>
+      </c>
+      <c r="F11" s="54">
+        <f t="shared" si="0"/>
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="100"/>
+      <c r="B12" s="101"/>
+      <c r="C12" s="100"/>
+      <c r="D12" s="100"/>
+      <c r="E12" s="102"/>
+      <c r="F12" s="102"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E17" s="98" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E18" s="99" t="s">
+        <v>156</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F19"/>
+  <sheetViews>
+    <sheetView view="pageBreakPreview" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" customWidth="1"/>
+    <col min="3" max="6" width="12" customWidth="1"/>
+    <col min="7" max="7" width="4.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="97" t="s">
+        <v>153</v>
+      </c>
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="97"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="95" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="95" t="s">
+        <v>91</v>
+      </c>
+      <c r="C3" s="95" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="95" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="95" t="s">
+        <v>59</v>
+      </c>
+      <c r="F3" s="95" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="38">
+        <v>1</v>
+      </c>
+      <c r="B4" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" s="38">
+        <v>25</v>
+      </c>
+      <c r="D4" s="38" t="s">
+        <v>89</v>
+      </c>
+      <c r="E4" s="54">
+        <f>VLOOKUP(B4,'daftar harga'!$B$4:$F$11,3)</f>
+        <v>6000</v>
+      </c>
+      <c r="F4" s="54">
+        <f>E4*C4</f>
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="38">
+        <v>2</v>
+      </c>
+      <c r="B5" s="38" t="s">
+        <v>61</v>
+      </c>
+      <c r="C5" s="38">
+        <v>25</v>
+      </c>
+      <c r="D5" s="38" t="s">
+        <v>89</v>
+      </c>
+      <c r="E5" s="54">
+        <f>VLOOKUP(B5,'daftar harga'!$B$4:$F$11,3)</f>
+        <v>6000</v>
+      </c>
+      <c r="F5" s="54">
+        <f>E5*C5</f>
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="38">
+        <v>3</v>
+      </c>
+      <c r="B6" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" s="38">
+        <v>25</v>
+      </c>
+      <c r="D6" s="38" t="s">
+        <v>89</v>
+      </c>
+      <c r="E6" s="54">
+        <f>VLOOKUP(B6,'daftar harga'!$B$4:$F$11,3)</f>
+        <v>6000</v>
+      </c>
+      <c r="F6" s="54">
+        <f>E6*C6</f>
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="38">
+        <v>4</v>
+      </c>
+      <c r="B7" s="38" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" s="38">
+        <v>13</v>
+      </c>
+      <c r="D7" s="38" t="s">
+        <v>90</v>
+      </c>
+      <c r="E7" s="54">
+        <f>VLOOKUP(B7,'daftar harga'!$B$4:$F$11,3)</f>
+        <v>16000</v>
+      </c>
+      <c r="F7" s="54">
+        <f>E7*C7</f>
+        <v>208000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="38">
+        <v>5</v>
+      </c>
+      <c r="B8" s="38" t="s">
+        <v>152</v>
+      </c>
+      <c r="C8" s="38">
+        <v>3</v>
+      </c>
+      <c r="D8" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="54">
+        <f>VLOOKUP(B8,'daftar harga'!$B$4:$F$11,3)</f>
+        <v>6000</v>
+      </c>
+      <c r="F8" s="54">
+        <f>E8*C8</f>
+        <v>18000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="38">
+        <v>6</v>
+      </c>
+      <c r="B9" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="38">
+        <v>8</v>
+      </c>
+      <c r="D9" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="54">
+        <f>VLOOKUP(B9,'daftar harga'!$B$4:$F$11,3)</f>
+        <v>11000</v>
+      </c>
+      <c r="F9" s="54">
+        <f>E9*C9</f>
+        <v>88000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="38">
+        <v>7</v>
+      </c>
+      <c r="B10" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" s="38">
+        <v>25</v>
+      </c>
+      <c r="D10" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="54">
+        <f>VLOOKUP(B10,'daftar harga'!$B$4:$F$11,3)</f>
+        <v>41000</v>
+      </c>
+      <c r="F10" s="54">
+        <f>E10*C10</f>
+        <v>1025000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="38">
+        <v>8</v>
+      </c>
+      <c r="B11" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" s="38">
+        <v>1</v>
+      </c>
+      <c r="D11" s="38" t="s">
+        <v>89</v>
+      </c>
+      <c r="E11" s="54">
+        <f>VLOOKUP(B11,'daftar harga'!$B$4:$F$11,3)</f>
+        <v>16000</v>
+      </c>
+      <c r="F11" s="54">
+        <f>E11*C11</f>
+        <v>16000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="38"/>
+      <c r="B12" s="38"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E18" s="98" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="19" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E19" s="99" t="s">
+        <v>156</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F18"/>
+  <sheetViews>
+    <sheetView view="pageBreakPreview" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" customWidth="1"/>
+    <col min="3" max="6" width="12" customWidth="1"/>
+    <col min="7" max="7" width="4.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="97" t="s">
+        <v>153</v>
+      </c>
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="97"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="95" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="95" t="s">
+        <v>91</v>
+      </c>
+      <c r="C3" s="95" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="95" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="95" t="s">
+        <v>59</v>
+      </c>
+      <c r="F3" s="95" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="38">
+        <v>1</v>
+      </c>
+      <c r="B4" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" s="38">
+        <v>25</v>
+      </c>
+      <c r="D4" s="38" t="s">
+        <v>89</v>
+      </c>
+      <c r="E4" s="54">
+        <f>VLOOKUP(B4,'daftar harga'!$B$4:$F$11,2)</f>
+        <v>5000</v>
+      </c>
+      <c r="F4" s="54">
+        <f>E4*C4</f>
+        <v>125000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="38">
+        <v>2</v>
+      </c>
+      <c r="B5" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="38">
+        <v>25</v>
+      </c>
+      <c r="D5" s="38" t="s">
+        <v>89</v>
+      </c>
+      <c r="E5" s="54">
+        <f>VLOOKUP(B5,'daftar harga'!$B$4:$F$11,2)</f>
+        <v>5000</v>
+      </c>
+      <c r="F5" s="54">
+        <f>E5*C5</f>
+        <v>125000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="38">
+        <v>3</v>
+      </c>
+      <c r="B6" s="38" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="38">
+        <v>13</v>
+      </c>
+      <c r="D6" s="38" t="s">
+        <v>90</v>
+      </c>
+      <c r="E6" s="54">
+        <f>VLOOKUP(B6,'daftar harga'!$B$4:$F$11,2)</f>
+        <v>15000</v>
+      </c>
+      <c r="F6" s="54">
+        <f>E6*C6</f>
+        <v>195000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="38">
+        <v>4</v>
+      </c>
+      <c r="B7" s="38" t="s">
+        <v>152</v>
+      </c>
+      <c r="C7" s="38">
+        <v>3</v>
+      </c>
+      <c r="D7" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="54">
+        <f>VLOOKUP(B7,'daftar harga'!$B$4:$F$11,2)</f>
+        <v>5000</v>
+      </c>
+      <c r="F7" s="54">
+        <f>E7*C7</f>
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="38">
+        <v>5</v>
+      </c>
+      <c r="B8" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" s="38">
+        <v>8</v>
+      </c>
+      <c r="D8" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="54">
+        <f>VLOOKUP(B8,'daftar harga'!$B$4:$F$11,2)</f>
+        <v>10000</v>
+      </c>
+      <c r="F8" s="54">
+        <f>E8*C8</f>
+        <v>80000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="38">
+        <v>6</v>
+      </c>
+      <c r="B9" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="C9" s="38">
+        <v>1</v>
+      </c>
+      <c r="D9" s="38" t="s">
+        <v>89</v>
+      </c>
+      <c r="E9" s="54">
+        <f>VLOOKUP(B9,'daftar harga'!$B$4:$F$11,2)</f>
+        <v>15000</v>
+      </c>
+      <c r="F9" s="54">
+        <f>E9*C9</f>
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="38">
+        <v>7</v>
+      </c>
+      <c r="B10" s="103" t="s">
+        <v>157</v>
+      </c>
+      <c r="C10" s="38">
+        <v>1</v>
+      </c>
+      <c r="D10" s="38" t="s">
+        <v>89</v>
+      </c>
+      <c r="E10" s="54">
+        <f>VLOOKUP(B10,'daftar harga'!$B$4:$F$11,2)</f>
+        <v>200000</v>
+      </c>
+      <c r="F10" s="54">
+        <f t="shared" ref="F10:F11" si="0">E10*C10</f>
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="38">
+        <v>8</v>
+      </c>
+      <c r="B11" s="103" t="s">
+        <v>158</v>
+      </c>
+      <c r="C11" s="38">
+        <v>1</v>
+      </c>
+      <c r="D11" s="38" t="s">
+        <v>89</v>
+      </c>
+      <c r="E11" s="54">
+        <f>VLOOKUP(B11,'daftar harga'!$B$4:$F$11,2)</f>
+        <v>5000</v>
+      </c>
+      <c r="F11" s="54">
+        <f t="shared" si="0"/>
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="100"/>
+      <c r="B12" s="101"/>
+      <c r="C12" s="100"/>
+      <c r="D12" s="100"/>
+      <c r="E12" s="102"/>
+      <c r="F12" s="102"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E17" s="98" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E18" s="99" t="s">
+        <v>156</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:E24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="18.140625" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" customWidth="1"/>
+    <col min="4" max="5" width="11.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="95" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="95" t="s">
+        <v>198</v>
+      </c>
+      <c r="C3" s="95" t="s">
+        <v>165</v>
+      </c>
+      <c r="D3" s="95" t="s">
+        <v>171</v>
+      </c>
+      <c r="E3" s="95" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="38">
+        <v>1</v>
+      </c>
+      <c r="B4" s="38" t="s">
+        <v>177</v>
+      </c>
+      <c r="C4" s="38" t="s">
+        <v>159</v>
+      </c>
+      <c r="D4" s="38" t="e">
+        <f>HLOOKUP(C4, 'daftar harga'!#REF!,2)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E4" s="38" t="e">
+        <f>HLOOKUP(C4, 'daftar harga'!#REF!,2)</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="38">
+        <v>2</v>
+      </c>
+      <c r="B5" s="38" t="s">
+        <v>178</v>
+      </c>
+      <c r="C5" s="38" t="s">
+        <v>160</v>
+      </c>
+      <c r="D5" s="38" t="e">
+        <f>HLOOKUP(C5, 'daftar harga'!#REF!,2)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E5" s="38" t="e">
+        <f>HLOOKUP(C5, 'daftar harga'!#REF!,2)</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="38">
+        <v>3</v>
+      </c>
+      <c r="B6" s="38" t="s">
+        <v>179</v>
+      </c>
+      <c r="C6" s="38" t="s">
+        <v>159</v>
+      </c>
+      <c r="D6" s="38" t="e">
+        <f>HLOOKUP(C6, 'daftar harga'!#REF!,2)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E6" s="38" t="e">
+        <f>HLOOKUP(C6, 'daftar harga'!#REF!,2)</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="38">
+        <v>4</v>
+      </c>
+      <c r="B7" s="38" t="s">
+        <v>180</v>
+      </c>
+      <c r="C7" s="38" t="s">
+        <v>163</v>
+      </c>
+      <c r="D7" s="38" t="e">
+        <f>HLOOKUP(C7, 'daftar harga'!#REF!,2)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E7" s="38" t="e">
+        <f>HLOOKUP(C7, 'daftar harga'!#REF!,2)</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="38">
+        <v>5</v>
+      </c>
+      <c r="B8" s="38" t="s">
+        <v>181</v>
+      </c>
+      <c r="C8" s="38" t="s">
+        <v>160</v>
+      </c>
+      <c r="D8" s="38" t="e">
+        <f>HLOOKUP(C8, 'daftar harga'!#REF!,2)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E8" s="38" t="e">
+        <f>HLOOKUP(C8, 'daftar harga'!#REF!,2)</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="38">
+        <v>6</v>
+      </c>
+      <c r="B9" s="38" t="s">
+        <v>182</v>
+      </c>
+      <c r="C9" s="38" t="s">
+        <v>159</v>
+      </c>
+      <c r="D9" s="38" t="e">
+        <f>HLOOKUP(C9, 'daftar harga'!#REF!,2)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E9" s="38" t="e">
+        <f>HLOOKUP(C9, 'daftar harga'!#REF!,2)</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="38">
+        <v>7</v>
+      </c>
+      <c r="B10" s="38" t="s">
+        <v>183</v>
+      </c>
+      <c r="C10" s="38" t="s">
+        <v>160</v>
+      </c>
+      <c r="D10" s="38" t="e">
+        <f>HLOOKUP(C10, 'daftar harga'!#REF!,2)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E10" s="38" t="e">
+        <f>HLOOKUP(C10, 'daftar harga'!#REF!,2)</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="38">
+        <v>8</v>
+      </c>
+      <c r="B11" s="38" t="s">
+        <v>184</v>
+      </c>
+      <c r="C11" s="38" t="s">
+        <v>162</v>
+      </c>
+      <c r="D11" s="38" t="e">
+        <f>HLOOKUP(C11, 'daftar harga'!#REF!,2)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E11" s="38" t="e">
+        <f>HLOOKUP(C11, 'daftar harga'!#REF!,2)</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="38">
+        <v>9</v>
+      </c>
+      <c r="B12" s="38" t="s">
+        <v>185</v>
+      </c>
+      <c r="C12" s="38" t="s">
+        <v>163</v>
+      </c>
+      <c r="D12" s="38" t="e">
+        <f>HLOOKUP(C12, 'daftar harga'!#REF!,2)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E12" s="38" t="e">
+        <f>HLOOKUP(C12, 'daftar harga'!#REF!,2)</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="38">
+        <v>10</v>
+      </c>
+      <c r="B13" s="38" t="s">
+        <v>186</v>
+      </c>
+      <c r="C13" s="38" t="s">
+        <v>161</v>
+      </c>
+      <c r="D13" s="38" t="e">
+        <f>HLOOKUP(C13, 'daftar harga'!#REF!,2)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E13" s="38" t="e">
+        <f>HLOOKUP(C13, 'daftar harga'!#REF!,2)</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="38">
+        <v>11</v>
+      </c>
+      <c r="B14" s="38" t="s">
+        <v>187</v>
+      </c>
+      <c r="C14" s="38" t="s">
+        <v>163</v>
+      </c>
+      <c r="D14" s="38" t="e">
+        <f>HLOOKUP(C14, 'daftar harga'!#REF!,2)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E14" s="38" t="e">
+        <f>HLOOKUP(C14, 'daftar harga'!#REF!,2)</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="38">
+        <v>12</v>
+      </c>
+      <c r="B15" s="38" t="s">
+        <v>188</v>
+      </c>
+      <c r="C15" s="38" t="s">
+        <v>163</v>
+      </c>
+      <c r="D15" s="38" t="e">
+        <f>HLOOKUP(C15, 'daftar harga'!#REF!,2)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E15" s="38" t="e">
+        <f>HLOOKUP(C15, 'daftar harga'!#REF!,2)</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="38">
+        <v>13</v>
+      </c>
+      <c r="B16" s="38" t="s">
+        <v>189</v>
+      </c>
+      <c r="C16" s="38" t="s">
+        <v>161</v>
+      </c>
+      <c r="D16" s="38" t="e">
+        <f>HLOOKUP(C16, 'daftar harga'!#REF!,2)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E16" s="38" t="e">
+        <f>HLOOKUP(C16, 'daftar harga'!#REF!,2)</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="38">
+        <v>14</v>
+      </c>
+      <c r="B17" s="38" t="s">
+        <v>190</v>
+      </c>
+      <c r="C17" s="38" t="s">
+        <v>160</v>
+      </c>
+      <c r="D17" s="38" t="e">
+        <f>HLOOKUP(C17, 'daftar harga'!#REF!,2)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E17" s="38" t="e">
+        <f>HLOOKUP(C17, 'daftar harga'!#REF!,2)</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="38">
+        <v>15</v>
+      </c>
+      <c r="B18" s="38" t="s">
+        <v>191</v>
+      </c>
+      <c r="C18" s="38" t="s">
+        <v>164</v>
+      </c>
+      <c r="D18" s="38" t="e">
+        <f>HLOOKUP(C18, 'daftar harga'!#REF!,2)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E18" s="38" t="e">
+        <f>HLOOKUP(C18, 'daftar harga'!#REF!,2)</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="38">
+        <v>16</v>
+      </c>
+      <c r="B19" s="38" t="s">
+        <v>192</v>
+      </c>
+      <c r="C19" s="38" t="s">
+        <v>163</v>
+      </c>
+      <c r="D19" s="38" t="e">
+        <f>HLOOKUP(C19, 'daftar harga'!#REF!,2)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E19" s="38" t="e">
+        <f>HLOOKUP(C19, 'daftar harga'!#REF!,2)</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="38">
+        <v>17</v>
+      </c>
+      <c r="B20" s="38" t="s">
+        <v>193</v>
+      </c>
+      <c r="C20" s="38" t="s">
+        <v>160</v>
+      </c>
+      <c r="D20" s="38" t="e">
+        <f>HLOOKUP(C20, 'daftar harga'!#REF!,2)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E20" s="38" t="e">
+        <f>HLOOKUP(C20, 'daftar harga'!#REF!,2)</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="38">
+        <v>18</v>
+      </c>
+      <c r="B21" s="38" t="s">
+        <v>194</v>
+      </c>
+      <c r="C21" s="38" t="s">
+        <v>159</v>
+      </c>
+      <c r="D21" s="38" t="e">
+        <f>HLOOKUP(C21, 'daftar harga'!#REF!,2)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E21" s="38" t="e">
+        <f>HLOOKUP(C21, 'daftar harga'!#REF!,2)</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="38">
+        <v>19</v>
+      </c>
+      <c r="B22" s="38" t="s">
+        <v>195</v>
+      </c>
+      <c r="C22" s="38" t="s">
+        <v>160</v>
+      </c>
+      <c r="D22" s="38" t="e">
+        <f>HLOOKUP(C22, 'daftar harga'!#REF!,2)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E22" s="38" t="e">
+        <f>HLOOKUP(C22, 'daftar harga'!#REF!,2)</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="38">
+        <v>20</v>
+      </c>
+      <c r="B23" s="38" t="s">
+        <v>196</v>
+      </c>
+      <c r="C23" s="38" t="s">
+        <v>163</v>
+      </c>
+      <c r="D23" s="38" t="e">
+        <f>HLOOKUP(C23, 'daftar harga'!#REF!,2)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E23" s="38" t="e">
+        <f>HLOOKUP(C23, 'daftar harga'!#REF!,2)</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="38">
+        <v>21</v>
+      </c>
+      <c r="B24" s="38" t="s">
+        <v>197</v>
+      </c>
+      <c r="C24" s="38" t="s">
+        <v>160</v>
+      </c>
+      <c r="D24" s="38" t="e">
+        <f>HLOOKUP(C24, 'daftar harga'!#REF!,2)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E24" s="38" t="e">
+        <f>HLOOKUP(C24, 'daftar harga'!#REF!,2)</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update hookup & v lookup
</commit_message>
<xml_diff>
--- a/LATIHAN EXCEL AHMADI.xlsx
+++ b/LATIHAN EXCEL AHMADI.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="13335" windowHeight="5130" firstSheet="5" activeTab="8"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="13335" windowHeight="5130" tabRatio="740" firstSheet="6" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="RPBMK FISTAN FISTUM" sheetId="4" r:id="rId1"/>
@@ -21,17 +21,20 @@
     <sheet name="kegiatan 3" sheetId="14" r:id="rId7"/>
     <sheet name="kegiatan 4" sheetId="15" r:id="rId8"/>
     <sheet name="penentuan baju" sheetId="13" r:id="rId9"/>
+    <sheet name="nilai vlookup" sheetId="16" r:id="rId10"/>
+    <sheet name="nilai hlookup" sheetId="17" r:id="rId11"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId10"/>
-    <externalReference r:id="rId11"/>
+    <externalReference r:id="rId12"/>
+    <externalReference r:id="rId13"/>
+    <externalReference r:id="rId14"/>
   </externalReferences>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="233">
   <si>
     <t>Satuan</t>
   </si>
@@ -628,6 +631,108 @@
   </si>
   <si>
     <t>Kegiatan</t>
+  </si>
+  <si>
+    <t>Peserta</t>
+  </si>
+  <si>
+    <t>Baju</t>
+  </si>
+  <si>
+    <t>NILAI RAPOR SMK NEGERI 1 KARANG BARU</t>
+  </si>
+  <si>
+    <t>TP. 2022/2023</t>
+  </si>
+  <si>
+    <t>KELAS</t>
+  </si>
+  <si>
+    <t>XI RPL 1</t>
+  </si>
+  <si>
+    <t>KKM : 76</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>NAMA</t>
+  </si>
+  <si>
+    <t>PENGETAHUAN</t>
+  </si>
+  <si>
+    <t>KETERAMPILAN</t>
+  </si>
+  <si>
+    <t>Rerata</t>
+  </si>
+  <si>
+    <t>Keterangan</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>RATA - RATA KELAS</t>
+  </si>
+  <si>
+    <t>Karang Baru,        Desember 2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Guru Mapel </t>
+  </si>
+  <si>
+    <t>Basis Data</t>
+  </si>
+  <si>
+    <t>Nip. 19860505 201403 1 003</t>
+  </si>
+  <si>
+    <t>76-80</t>
+  </si>
+  <si>
+    <t>81-85</t>
+  </si>
+  <si>
+    <t>86-90</t>
+  </si>
+  <si>
+    <t>90-95</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>TL</t>
+  </si>
+  <si>
+    <t>Range</t>
+  </si>
+  <si>
+    <t>96-100</t>
+  </si>
+  <si>
+    <t>70-75</t>
+  </si>
+  <si>
+    <t>Mutu</t>
+  </si>
+  <si>
+    <t>Nilai</t>
+  </si>
+  <si>
+    <t>Dummy</t>
   </si>
 </sst>
 </file>
@@ -639,7 +744,7 @@
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -754,8 +859,14 @@
       <charset val="1"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -786,8 +897,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -867,6 +996,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -874,7 +1029,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="130">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1101,48 +1256,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1161,6 +1274,118 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="16" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1234,6 +1459,154 @@
           </cell>
         </row>
       </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="peserta"/>
+      <sheetName val="project database"/>
+      <sheetName val="piket"/>
+      <sheetName val="project Vidio"/>
+      <sheetName val="project 1"/>
+      <sheetName val="ABSENSI"/>
+      <sheetName val="Sikap"/>
+      <sheetName val="projekakhir"/>
+      <sheetName val="Pengetahuan"/>
+      <sheetName val="Pengetahuan (2)"/>
+      <sheetName val="Keterampilan"/>
+      <sheetName val="CETAK NILAI RAPOR"/>
+      <sheetName val="CATATAN SK"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8">
+        <row r="6">
+          <cell r="B6" t="str">
+            <v>Adita Dwi Rezeki P</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="B7" t="str">
+            <v>Aditya Gufran</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="B8" t="str">
+            <v>Al Adlu Vitrah</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="B9" t="str">
+            <v>Aulia Rahman</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="B10" t="str">
+            <v>Bunga Azza Delia</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="B11" t="str">
+            <v>Celci Monica</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="B12" t="str">
+            <v>Dea Selpina</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="B13" t="str">
+            <v>Dzamar Rahim</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="B14" t="str">
+            <v>Indah Rahayu</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="B15" t="str">
+            <v>Jihan Raihanah</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="B16" t="str">
+            <v>M. Fahri</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="B17" t="str">
+            <v>M. Rifki</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="B18" t="str">
+            <v>M. Sulthan Khair</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="B19" t="str">
+            <v>Nabila Putri</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="B20" t="str">
+            <v>Putri Amelia</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="B21" t="str">
+            <v>Rina Ramadani</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="B22" t="str">
+            <v>Ryan Fahlevi</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="B23" t="str">
+            <v>Sherly Amanda Elysia</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="B24" t="str">
+            <v>Sri Ariyani</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="B25" t="str">
+            <v>T. Amylia Safitri</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="B26" t="str">
+            <v>Windi Safira</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="B27" t="str">
+            <v>Zahwa Maila Puspita</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1532,7 +1905,7 @@
   <dimension ref="A1:M93"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1553,58 +1926,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="110" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82" t="s">
+      <c r="B1" s="110"/>
+      <c r="C1" s="110"/>
+      <c r="D1" s="110"/>
+      <c r="E1" s="110"/>
+      <c r="F1" s="110"/>
+      <c r="G1" s="110" t="s">
         <v>58</v>
       </c>
-      <c r="H1" s="82"/>
-      <c r="I1" s="82"/>
-      <c r="J1" s="82"/>
-      <c r="K1" s="82"/>
-      <c r="L1" s="82"/>
+      <c r="H1" s="110"/>
+      <c r="I1" s="110"/>
+      <c r="J1" s="110"/>
+      <c r="K1" s="110"/>
+      <c r="L1" s="110"/>
     </row>
     <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="82" t="s">
+      <c r="A2" s="110" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="82"/>
-      <c r="C2" s="82"/>
-      <c r="D2" s="82"/>
-      <c r="E2" s="82"/>
-      <c r="F2" s="82"/>
-      <c r="G2" s="82" t="s">
+      <c r="B2" s="110"/>
+      <c r="C2" s="110"/>
+      <c r="D2" s="110"/>
+      <c r="E2" s="110"/>
+      <c r="F2" s="110"/>
+      <c r="G2" s="110" t="s">
         <v>36</v>
       </c>
-      <c r="H2" s="82"/>
-      <c r="I2" s="82"/>
-      <c r="J2" s="82"/>
-      <c r="K2" s="82"/>
-      <c r="L2" s="82"/>
+      <c r="H2" s="110"/>
+      <c r="I2" s="110"/>
+      <c r="J2" s="110"/>
+      <c r="K2" s="110"/>
+      <c r="L2" s="110"/>
     </row>
     <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="82" t="s">
+      <c r="A3" s="110" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="82"/>
-      <c r="C3" s="82"/>
-      <c r="D3" s="82"/>
-      <c r="E3" s="82"/>
-      <c r="F3" s="82"/>
-      <c r="G3" s="82" t="s">
+      <c r="B3" s="110"/>
+      <c r="C3" s="110"/>
+      <c r="D3" s="110"/>
+      <c r="E3" s="110"/>
+      <c r="F3" s="110"/>
+      <c r="G3" s="110" t="s">
         <v>35</v>
       </c>
-      <c r="H3" s="82"/>
-      <c r="I3" s="82"/>
-      <c r="J3" s="82"/>
-      <c r="K3" s="82"/>
-      <c r="L3" s="82"/>
+      <c r="H3" s="110"/>
+      <c r="I3" s="110"/>
+      <c r="J3" s="110"/>
+      <c r="K3" s="110"/>
+      <c r="L3" s="110"/>
     </row>
     <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E4" s="1"/>
@@ -1613,14 +1986,14 @@
       <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="81" t="s">
+      <c r="A6" s="111" t="s">
         <v>57</v>
       </c>
-      <c r="B6" s="81"/>
-      <c r="C6" s="81"/>
-      <c r="D6" s="81"/>
-      <c r="E6" s="81"/>
-      <c r="F6" s="81"/>
+      <c r="B6" s="111"/>
+      <c r="C6" s="111"/>
+      <c r="D6" s="111"/>
+      <c r="E6" s="111"/>
+      <c r="F6" s="111"/>
       <c r="G6" s="20" t="s">
         <v>4</v>
       </c>
@@ -3042,61 +3415,61 @@
       <c r="L61" s="11"/>
     </row>
     <row r="62" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="82" t="s">
+      <c r="A62" s="110" t="s">
         <v>38</v>
       </c>
-      <c r="B62" s="82"/>
-      <c r="C62" s="82"/>
-      <c r="D62" s="82"/>
-      <c r="E62" s="82"/>
-      <c r="F62" s="82"/>
-      <c r="G62" s="82" t="s">
+      <c r="B62" s="110"/>
+      <c r="C62" s="110"/>
+      <c r="D62" s="110"/>
+      <c r="E62" s="110"/>
+      <c r="F62" s="110"/>
+      <c r="G62" s="110" t="s">
         <v>37</v>
       </c>
-      <c r="H62" s="82"/>
-      <c r="I62" s="82"/>
-      <c r="J62" s="82"/>
-      <c r="K62" s="82"/>
-      <c r="L62" s="82"/>
-      <c r="M62" s="82"/>
+      <c r="H62" s="110"/>
+      <c r="I62" s="110"/>
+      <c r="J62" s="110"/>
+      <c r="K62" s="110"/>
+      <c r="L62" s="110"/>
+      <c r="M62" s="110"/>
     </row>
     <row r="63" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="82" t="s">
+      <c r="A63" s="110" t="s">
         <v>36</v>
       </c>
-      <c r="B63" s="82"/>
-      <c r="C63" s="82"/>
-      <c r="D63" s="82"/>
-      <c r="E63" s="82"/>
-      <c r="F63" s="82"/>
-      <c r="G63" s="82" t="s">
+      <c r="B63" s="110"/>
+      <c r="C63" s="110"/>
+      <c r="D63" s="110"/>
+      <c r="E63" s="110"/>
+      <c r="F63" s="110"/>
+      <c r="G63" s="110" t="s">
         <v>36</v>
       </c>
-      <c r="H63" s="82"/>
-      <c r="I63" s="82"/>
-      <c r="J63" s="82"/>
-      <c r="K63" s="82"/>
-      <c r="L63" s="82"/>
-      <c r="M63" s="82"/>
+      <c r="H63" s="110"/>
+      <c r="I63" s="110"/>
+      <c r="J63" s="110"/>
+      <c r="K63" s="110"/>
+      <c r="L63" s="110"/>
+      <c r="M63" s="110"/>
     </row>
     <row r="64" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="82" t="s">
+      <c r="A64" s="110" t="s">
         <v>35</v>
       </c>
-      <c r="B64" s="82"/>
-      <c r="C64" s="82"/>
-      <c r="D64" s="82"/>
-      <c r="E64" s="82"/>
-      <c r="F64" s="82"/>
-      <c r="G64" s="82" t="s">
+      <c r="B64" s="110"/>
+      <c r="C64" s="110"/>
+      <c r="D64" s="110"/>
+      <c r="E64" s="110"/>
+      <c r="F64" s="110"/>
+      <c r="G64" s="110" t="s">
         <v>35</v>
       </c>
-      <c r="H64" s="82"/>
-      <c r="I64" s="82"/>
-      <c r="J64" s="82"/>
-      <c r="K64" s="82"/>
-      <c r="L64" s="82"/>
-      <c r="M64" s="82"/>
+      <c r="H64" s="110"/>
+      <c r="I64" s="110"/>
+      <c r="J64" s="110"/>
+      <c r="K64" s="110"/>
+      <c r="L64" s="110"/>
+      <c r="M64" s="110"/>
     </row>
     <row r="65" spans="1:13" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="27"/>
@@ -3111,14 +3484,14 @@
       <c r="L65" s="1"/>
     </row>
     <row r="66" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="81" t="s">
+      <c r="A66" s="111" t="s">
         <v>34</v>
       </c>
-      <c r="B66" s="81"/>
-      <c r="C66" s="81"/>
-      <c r="D66" s="81"/>
-      <c r="E66" s="81"/>
-      <c r="F66" s="81"/>
+      <c r="B66" s="111"/>
+      <c r="C66" s="111"/>
+      <c r="D66" s="111"/>
+      <c r="E66" s="111"/>
+      <c r="F66" s="111"/>
     </row>
     <row r="67" spans="1:13" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="10" t="s">
@@ -3345,14 +3718,14 @@
       </c>
     </row>
     <row r="72" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="81" t="s">
+      <c r="A72" s="111" t="s">
         <v>24</v>
       </c>
-      <c r="B72" s="81"/>
-      <c r="C72" s="81"/>
-      <c r="D72" s="81"/>
-      <c r="E72" s="81"/>
-      <c r="F72" s="81"/>
+      <c r="B72" s="111"/>
+      <c r="C72" s="111"/>
+      <c r="D72" s="111"/>
+      <c r="E72" s="111"/>
+      <c r="F72" s="111"/>
     </row>
     <row r="73" spans="1:13" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="10" t="s">
@@ -3461,14 +3834,14 @@
       <c r="G77" s="5"/>
     </row>
     <row r="78" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="81" t="s">
+      <c r="A78" s="111" t="s">
         <v>23</v>
       </c>
-      <c r="B78" s="81"/>
-      <c r="C78" s="81"/>
-      <c r="D78" s="81"/>
-      <c r="E78" s="81"/>
-      <c r="F78" s="81"/>
+      <c r="B78" s="111"/>
+      <c r="C78" s="111"/>
+      <c r="D78" s="111"/>
+      <c r="E78" s="111"/>
+      <c r="F78" s="111"/>
     </row>
     <row r="79" spans="1:13" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="10" t="s">
@@ -3584,25 +3957,1756 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A78:F78"/>
+    <mergeCell ref="A72:F72"/>
+    <mergeCell ref="A66:F66"/>
+    <mergeCell ref="G64:M64"/>
+    <mergeCell ref="G63:M63"/>
+    <mergeCell ref="G62:M62"/>
+    <mergeCell ref="A64:F64"/>
+    <mergeCell ref="A62:F62"/>
+    <mergeCell ref="A63:F63"/>
+    <mergeCell ref="A6:F6"/>
     <mergeCell ref="G1:L1"/>
     <mergeCell ref="G2:L2"/>
     <mergeCell ref="G3:L3"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A3:F3"/>
-    <mergeCell ref="G62:M62"/>
-    <mergeCell ref="A64:F64"/>
-    <mergeCell ref="A62:F62"/>
-    <mergeCell ref="A63:F63"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="A78:F78"/>
-    <mergeCell ref="A72:F72"/>
-    <mergeCell ref="A66:F66"/>
-    <mergeCell ref="G64:M64"/>
-    <mergeCell ref="G63:M63"/>
   </mergeCells>
   <pageMargins left="0.56000000000000005" right="0.3" top="0.57999999999999996" bottom="0.53" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7:G28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.7109375" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" customWidth="1"/>
+    <col min="3" max="5" width="5.140625" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="127" t="s">
+        <v>201</v>
+      </c>
+      <c r="B1" s="127"/>
+      <c r="C1" s="127"/>
+      <c r="D1" s="127"/>
+      <c r="E1" s="83"/>
+      <c r="F1" s="83"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="127" t="s">
+        <v>202</v>
+      </c>
+      <c r="B2" s="127"/>
+      <c r="C2" s="127"/>
+      <c r="D2" s="127"/>
+      <c r="E2" s="83"/>
+      <c r="F2" s="83"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="93" t="s">
+        <v>203</v>
+      </c>
+      <c r="B4" s="93" t="s">
+        <v>204</v>
+      </c>
+      <c r="C4" s="93"/>
+      <c r="D4" s="93" t="s">
+        <v>205</v>
+      </c>
+      <c r="E4" s="93" t="s">
+        <v>205</v>
+      </c>
+      <c r="F4" s="93" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="93"/>
+      <c r="B5" s="93"/>
+      <c r="C5" s="93"/>
+      <c r="D5" s="93"/>
+      <c r="E5" s="93"/>
+      <c r="F5" s="93"/>
+    </row>
+    <row r="6" spans="1:11" ht="66.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="94" t="s">
+        <v>206</v>
+      </c>
+      <c r="B6" s="94" t="s">
+        <v>207</v>
+      </c>
+      <c r="C6" s="94" t="s">
+        <v>208</v>
+      </c>
+      <c r="D6" s="109" t="s">
+        <v>209</v>
+      </c>
+      <c r="E6" s="109" t="s">
+        <v>210</v>
+      </c>
+      <c r="F6" s="109" t="s">
+        <v>210</v>
+      </c>
+      <c r="G6" s="109" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="95">
+        <v>1</v>
+      </c>
+      <c r="B7" s="96" t="str">
+        <f>[3]Pengetahuan!B6</f>
+        <v>Adita Dwi Rezeki P</v>
+      </c>
+      <c r="C7" s="97">
+        <v>95</v>
+      </c>
+      <c r="D7" s="107">
+        <v>80</v>
+      </c>
+      <c r="E7" s="98">
+        <f>AVERAGE(C7:D7)</f>
+        <v>87.5</v>
+      </c>
+      <c r="F7" s="98" t="str">
+        <f>VLOOKUP(E7,$I$7:$K$13,3,TRUE)</f>
+        <v>C</v>
+      </c>
+      <c r="G7" s="108" t="str">
+        <f>IF(E7&gt;=76,"Aman",IF(E7&lt;76,"Remed",))</f>
+        <v>Aman</v>
+      </c>
+      <c r="J7" s="92" t="s">
+        <v>227</v>
+      </c>
+      <c r="K7" s="92" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="95">
+        <v>2</v>
+      </c>
+      <c r="B8" s="96" t="str">
+        <f>[3]Pengetahuan!B7</f>
+        <v>Aditya Gufran</v>
+      </c>
+      <c r="C8" s="97">
+        <v>95</v>
+      </c>
+      <c r="D8" s="107">
+        <v>80</v>
+      </c>
+      <c r="E8" s="98">
+        <f t="shared" ref="E8:E28" si="0">AVERAGE(C8:D8)</f>
+        <v>87.5</v>
+      </c>
+      <c r="F8" s="98" t="str">
+        <f t="shared" ref="F8:F28" si="1">VLOOKUP(E8,$I$7:$K$13,3,TRUE)</f>
+        <v>C</v>
+      </c>
+      <c r="G8" s="108" t="str">
+        <f t="shared" ref="G8:G28" si="2">IF(E8&gt;=76,"Aman",IF(E8&lt;76,"Remed",))</f>
+        <v>Aman</v>
+      </c>
+      <c r="I8">
+        <v>70</v>
+      </c>
+      <c r="J8" s="82" t="s">
+        <v>229</v>
+      </c>
+      <c r="K8" s="82" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="95">
+        <v>3</v>
+      </c>
+      <c r="B9" s="96" t="str">
+        <f>[3]Pengetahuan!B8</f>
+        <v>Al Adlu Vitrah</v>
+      </c>
+      <c r="C9" s="97">
+        <v>95</v>
+      </c>
+      <c r="D9" s="107">
+        <v>80</v>
+      </c>
+      <c r="E9" s="98">
+        <f t="shared" si="0"/>
+        <v>87.5</v>
+      </c>
+      <c r="F9" s="98" t="str">
+        <f t="shared" si="1"/>
+        <v>C</v>
+      </c>
+      <c r="G9" s="108" t="str">
+        <f t="shared" si="2"/>
+        <v>Aman</v>
+      </c>
+      <c r="I9">
+        <v>76</v>
+      </c>
+      <c r="J9" s="82" t="s">
+        <v>218</v>
+      </c>
+      <c r="K9" s="82" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="95">
+        <v>4</v>
+      </c>
+      <c r="B10" s="96" t="str">
+        <f>[3]Pengetahuan!B9</f>
+        <v>Aulia Rahman</v>
+      </c>
+      <c r="C10" s="97">
+        <v>95</v>
+      </c>
+      <c r="D10" s="107">
+        <v>80</v>
+      </c>
+      <c r="E10" s="98">
+        <f t="shared" si="0"/>
+        <v>87.5</v>
+      </c>
+      <c r="F10" s="98" t="str">
+        <f t="shared" si="1"/>
+        <v>C</v>
+      </c>
+      <c r="G10" s="108" t="str">
+        <f t="shared" si="2"/>
+        <v>Aman</v>
+      </c>
+      <c r="I10">
+        <v>81</v>
+      </c>
+      <c r="J10" s="82" t="s">
+        <v>219</v>
+      </c>
+      <c r="K10" s="82" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="95">
+        <v>5</v>
+      </c>
+      <c r="B11" s="96" t="str">
+        <f>[3]Pengetahuan!B10</f>
+        <v>Bunga Azza Delia</v>
+      </c>
+      <c r="C11" s="97">
+        <v>95</v>
+      </c>
+      <c r="D11" s="107">
+        <v>80</v>
+      </c>
+      <c r="E11" s="98">
+        <f t="shared" si="0"/>
+        <v>87.5</v>
+      </c>
+      <c r="F11" s="98" t="str">
+        <f t="shared" si="1"/>
+        <v>C</v>
+      </c>
+      <c r="G11" s="108" t="str">
+        <f t="shared" si="2"/>
+        <v>Aman</v>
+      </c>
+      <c r="I11">
+        <v>86</v>
+      </c>
+      <c r="J11" s="82" t="s">
+        <v>220</v>
+      </c>
+      <c r="K11" s="82" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="95">
+        <v>6</v>
+      </c>
+      <c r="B12" s="96" t="str">
+        <f>[3]Pengetahuan!B11</f>
+        <v>Celci Monica</v>
+      </c>
+      <c r="C12" s="97">
+        <v>95</v>
+      </c>
+      <c r="D12" s="107">
+        <v>80</v>
+      </c>
+      <c r="E12" s="98">
+        <f t="shared" si="0"/>
+        <v>87.5</v>
+      </c>
+      <c r="F12" s="98" t="str">
+        <f t="shared" si="1"/>
+        <v>C</v>
+      </c>
+      <c r="G12" s="108" t="str">
+        <f t="shared" si="2"/>
+        <v>Aman</v>
+      </c>
+      <c r="I12">
+        <v>90</v>
+      </c>
+      <c r="J12" s="82" t="s">
+        <v>221</v>
+      </c>
+      <c r="K12" s="82" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="95">
+        <v>7</v>
+      </c>
+      <c r="B13" s="96" t="str">
+        <f>[3]Pengetahuan!B12</f>
+        <v>Dea Selpina</v>
+      </c>
+      <c r="C13" s="97">
+        <v>95</v>
+      </c>
+      <c r="D13" s="107">
+        <v>80</v>
+      </c>
+      <c r="E13" s="98">
+        <f t="shared" si="0"/>
+        <v>87.5</v>
+      </c>
+      <c r="F13" s="98" t="str">
+        <f t="shared" si="1"/>
+        <v>C</v>
+      </c>
+      <c r="G13" s="108" t="str">
+        <f t="shared" si="2"/>
+        <v>Aman</v>
+      </c>
+      <c r="I13">
+        <v>96</v>
+      </c>
+      <c r="J13" s="82" t="s">
+        <v>228</v>
+      </c>
+      <c r="K13" s="82" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="95">
+        <v>8</v>
+      </c>
+      <c r="B14" s="96" t="str">
+        <f>[3]Pengetahuan!B13</f>
+        <v>Dzamar Rahim</v>
+      </c>
+      <c r="C14" s="97">
+        <v>95</v>
+      </c>
+      <c r="D14" s="107">
+        <v>80</v>
+      </c>
+      <c r="E14" s="98">
+        <f t="shared" si="0"/>
+        <v>87.5</v>
+      </c>
+      <c r="F14" s="98" t="str">
+        <f t="shared" si="1"/>
+        <v>C</v>
+      </c>
+      <c r="G14" s="108" t="str">
+        <f t="shared" si="2"/>
+        <v>Aman</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="95">
+        <v>9</v>
+      </c>
+      <c r="B15" s="96" t="str">
+        <f>[3]Pengetahuan!B14</f>
+        <v>Indah Rahayu</v>
+      </c>
+      <c r="C15" s="97">
+        <v>95</v>
+      </c>
+      <c r="D15" s="107">
+        <v>80</v>
+      </c>
+      <c r="E15" s="98">
+        <f t="shared" si="0"/>
+        <v>87.5</v>
+      </c>
+      <c r="F15" s="98" t="str">
+        <f t="shared" si="1"/>
+        <v>C</v>
+      </c>
+      <c r="G15" s="108" t="str">
+        <f t="shared" si="2"/>
+        <v>Aman</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="95">
+        <v>10</v>
+      </c>
+      <c r="B16" s="96" t="str">
+        <f>[3]Pengetahuan!B15</f>
+        <v>Jihan Raihanah</v>
+      </c>
+      <c r="C16" s="97">
+        <v>95</v>
+      </c>
+      <c r="D16" s="107">
+        <v>80</v>
+      </c>
+      <c r="E16" s="98">
+        <f t="shared" si="0"/>
+        <v>87.5</v>
+      </c>
+      <c r="F16" s="98" t="str">
+        <f t="shared" si="1"/>
+        <v>C</v>
+      </c>
+      <c r="G16" s="108" t="str">
+        <f t="shared" si="2"/>
+        <v>Aman</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="95">
+        <v>11</v>
+      </c>
+      <c r="B17" s="96" t="str">
+        <f>[3]Pengetahuan!B16</f>
+        <v>M. Fahri</v>
+      </c>
+      <c r="C17" s="97">
+        <v>95</v>
+      </c>
+      <c r="D17" s="107">
+        <v>80</v>
+      </c>
+      <c r="E17" s="98">
+        <f t="shared" si="0"/>
+        <v>87.5</v>
+      </c>
+      <c r="F17" s="98" t="str">
+        <f t="shared" si="1"/>
+        <v>C</v>
+      </c>
+      <c r="G17" s="108" t="str">
+        <f t="shared" si="2"/>
+        <v>Aman</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="95">
+        <v>12</v>
+      </c>
+      <c r="B18" s="96" t="str">
+        <f>[3]Pengetahuan!B17</f>
+        <v>M. Rifki</v>
+      </c>
+      <c r="C18" s="97">
+        <v>95</v>
+      </c>
+      <c r="D18" s="107">
+        <v>80</v>
+      </c>
+      <c r="E18" s="98">
+        <f t="shared" si="0"/>
+        <v>87.5</v>
+      </c>
+      <c r="F18" s="98" t="str">
+        <f t="shared" si="1"/>
+        <v>C</v>
+      </c>
+      <c r="G18" s="108" t="str">
+        <f t="shared" si="2"/>
+        <v>Aman</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="95">
+        <v>13</v>
+      </c>
+      <c r="B19" s="96" t="str">
+        <f>[3]Pengetahuan!B18</f>
+        <v>M. Sulthan Khair</v>
+      </c>
+      <c r="C19" s="97">
+        <v>95</v>
+      </c>
+      <c r="D19" s="107">
+        <v>80</v>
+      </c>
+      <c r="E19" s="98">
+        <f t="shared" si="0"/>
+        <v>87.5</v>
+      </c>
+      <c r="F19" s="98" t="str">
+        <f t="shared" si="1"/>
+        <v>C</v>
+      </c>
+      <c r="G19" s="108" t="str">
+        <f t="shared" si="2"/>
+        <v>Aman</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="95">
+        <v>14</v>
+      </c>
+      <c r="B20" s="96" t="str">
+        <f>[3]Pengetahuan!B19</f>
+        <v>Nabila Putri</v>
+      </c>
+      <c r="C20" s="97">
+        <v>95</v>
+      </c>
+      <c r="D20" s="107">
+        <v>80</v>
+      </c>
+      <c r="E20" s="98">
+        <f t="shared" si="0"/>
+        <v>87.5</v>
+      </c>
+      <c r="F20" s="98" t="str">
+        <f t="shared" si="1"/>
+        <v>C</v>
+      </c>
+      <c r="G20" s="108" t="str">
+        <f t="shared" si="2"/>
+        <v>Aman</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="95">
+        <v>15</v>
+      </c>
+      <c r="B21" s="96" t="str">
+        <f>[3]Pengetahuan!B20</f>
+        <v>Putri Amelia</v>
+      </c>
+      <c r="C21" s="97">
+        <v>95</v>
+      </c>
+      <c r="D21" s="107">
+        <v>80</v>
+      </c>
+      <c r="E21" s="98">
+        <f t="shared" si="0"/>
+        <v>87.5</v>
+      </c>
+      <c r="F21" s="98" t="str">
+        <f t="shared" si="1"/>
+        <v>C</v>
+      </c>
+      <c r="G21" s="108" t="str">
+        <f t="shared" si="2"/>
+        <v>Aman</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="95">
+        <v>16</v>
+      </c>
+      <c r="B22" s="96" t="str">
+        <f>[3]Pengetahuan!B21</f>
+        <v>Rina Ramadani</v>
+      </c>
+      <c r="C22" s="97">
+        <v>95</v>
+      </c>
+      <c r="D22" s="107">
+        <v>80</v>
+      </c>
+      <c r="E22" s="98">
+        <f t="shared" si="0"/>
+        <v>87.5</v>
+      </c>
+      <c r="F22" s="98" t="str">
+        <f t="shared" si="1"/>
+        <v>C</v>
+      </c>
+      <c r="G22" s="108" t="str">
+        <f t="shared" si="2"/>
+        <v>Aman</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="95">
+        <v>17</v>
+      </c>
+      <c r="B23" s="96" t="str">
+        <f>[3]Pengetahuan!B22</f>
+        <v>Ryan Fahlevi</v>
+      </c>
+      <c r="C23" s="97">
+        <v>95</v>
+      </c>
+      <c r="D23" s="107">
+        <v>80</v>
+      </c>
+      <c r="E23" s="98">
+        <f t="shared" si="0"/>
+        <v>87.5</v>
+      </c>
+      <c r="F23" s="98" t="str">
+        <f t="shared" si="1"/>
+        <v>C</v>
+      </c>
+      <c r="G23" s="108" t="str">
+        <f t="shared" si="2"/>
+        <v>Aman</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="95">
+        <v>18</v>
+      </c>
+      <c r="B24" s="96" t="str">
+        <f>[3]Pengetahuan!B23</f>
+        <v>Sherly Amanda Elysia</v>
+      </c>
+      <c r="C24" s="97">
+        <v>95</v>
+      </c>
+      <c r="D24" s="107">
+        <v>80</v>
+      </c>
+      <c r="E24" s="98">
+        <f t="shared" si="0"/>
+        <v>87.5</v>
+      </c>
+      <c r="F24" s="98" t="str">
+        <f t="shared" si="1"/>
+        <v>C</v>
+      </c>
+      <c r="G24" s="108" t="str">
+        <f t="shared" si="2"/>
+        <v>Aman</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="95">
+        <v>19</v>
+      </c>
+      <c r="B25" s="96" t="str">
+        <f>[3]Pengetahuan!B24</f>
+        <v>Sri Ariyani</v>
+      </c>
+      <c r="C25" s="97">
+        <v>95</v>
+      </c>
+      <c r="D25" s="107">
+        <v>80</v>
+      </c>
+      <c r="E25" s="98">
+        <f t="shared" si="0"/>
+        <v>87.5</v>
+      </c>
+      <c r="F25" s="98" t="str">
+        <f t="shared" si="1"/>
+        <v>C</v>
+      </c>
+      <c r="G25" s="108" t="str">
+        <f t="shared" si="2"/>
+        <v>Aman</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="95">
+        <v>20</v>
+      </c>
+      <c r="B26" s="96" t="str">
+        <f>[3]Pengetahuan!B25</f>
+        <v>T. Amylia Safitri</v>
+      </c>
+      <c r="C26" s="97">
+        <v>95</v>
+      </c>
+      <c r="D26" s="107">
+        <v>80</v>
+      </c>
+      <c r="E26" s="98">
+        <f t="shared" si="0"/>
+        <v>87.5</v>
+      </c>
+      <c r="F26" s="98" t="str">
+        <f t="shared" si="1"/>
+        <v>C</v>
+      </c>
+      <c r="G26" s="108" t="str">
+        <f t="shared" si="2"/>
+        <v>Aman</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="95">
+        <v>21</v>
+      </c>
+      <c r="B27" s="96" t="str">
+        <f>[3]Pengetahuan!B26</f>
+        <v>Windi Safira</v>
+      </c>
+      <c r="C27" s="97">
+        <v>95</v>
+      </c>
+      <c r="D27" s="107">
+        <v>80</v>
+      </c>
+      <c r="E27" s="98">
+        <f t="shared" si="0"/>
+        <v>87.5</v>
+      </c>
+      <c r="F27" s="98" t="str">
+        <f t="shared" si="1"/>
+        <v>C</v>
+      </c>
+      <c r="G27" s="108" t="str">
+        <f t="shared" si="2"/>
+        <v>Aman</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="95">
+        <v>22</v>
+      </c>
+      <c r="B28" s="96" t="str">
+        <f>[3]Pengetahuan!B27</f>
+        <v>Zahwa Maila Puspita</v>
+      </c>
+      <c r="C28" s="97">
+        <v>95</v>
+      </c>
+      <c r="D28" s="107">
+        <v>80</v>
+      </c>
+      <c r="E28" s="98">
+        <f t="shared" si="0"/>
+        <v>87.5</v>
+      </c>
+      <c r="F28" s="98" t="str">
+        <f t="shared" si="1"/>
+        <v>C</v>
+      </c>
+      <c r="G28" s="108" t="str">
+        <f t="shared" si="2"/>
+        <v>Aman</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="99"/>
+      <c r="B29" s="100"/>
+      <c r="C29" s="101"/>
+      <c r="D29" s="101"/>
+      <c r="E29" s="101"/>
+      <c r="F29" s="101"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="99"/>
+      <c r="B30" s="100"/>
+      <c r="C30" s="101"/>
+      <c r="D30" s="101"/>
+      <c r="E30" s="101"/>
+      <c r="F30" s="101"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="102"/>
+      <c r="B31" s="102" t="s">
+        <v>213</v>
+      </c>
+      <c r="C31" s="103">
+        <f>AVERAGE(C7:C30)</f>
+        <v>95</v>
+      </c>
+      <c r="D31" s="103">
+        <f>AVERAGE(D7:D30)</f>
+        <v>80</v>
+      </c>
+      <c r="E31" s="103">
+        <f>AVERAGE(E7:E30)</f>
+        <v>87.5</v>
+      </c>
+      <c r="F31" s="103" t="e">
+        <f>AVERAGE(F7:F30)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G31" s="104">
+        <f>COUNTIF(G7:G28,"Remed")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="99"/>
+      <c r="B32" s="99"/>
+      <c r="C32" s="101"/>
+      <c r="D32" s="101"/>
+      <c r="E32" s="101"/>
+      <c r="F32" s="101"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="93"/>
+      <c r="B33" s="93"/>
+      <c r="C33" s="93" t="s">
+        <v>214</v>
+      </c>
+      <c r="D33" s="93"/>
+      <c r="E33" s="93"/>
+      <c r="F33" s="93"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="93"/>
+      <c r="B34" s="93"/>
+      <c r="C34" s="93" t="s">
+        <v>215</v>
+      </c>
+      <c r="D34" s="93" t="s">
+        <v>216</v>
+      </c>
+      <c r="E34" s="93" t="s">
+        <v>216</v>
+      </c>
+      <c r="F34" s="93" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="93"/>
+      <c r="B35" s="93"/>
+      <c r="C35" s="93"/>
+      <c r="D35" s="93"/>
+      <c r="E35" s="93"/>
+      <c r="F35" s="93"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="93"/>
+      <c r="B36" s="93"/>
+      <c r="C36" s="93"/>
+      <c r="D36" s="93"/>
+      <c r="E36" s="93"/>
+      <c r="F36" s="93"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="93"/>
+      <c r="B37" s="93"/>
+      <c r="C37" s="128" t="s">
+        <v>155</v>
+      </c>
+      <c r="D37" s="128"/>
+      <c r="E37" s="105"/>
+      <c r="F37" s="105"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="93"/>
+      <c r="B38" s="93"/>
+      <c r="C38" s="129" t="s">
+        <v>217</v>
+      </c>
+      <c r="D38" s="129"/>
+      <c r="E38" s="106"/>
+      <c r="F38" s="106"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C38:D38"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O38"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.7109375" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" customWidth="1"/>
+    <col min="3" max="5" width="5.140625" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="127" t="s">
+        <v>201</v>
+      </c>
+      <c r="B1" s="127"/>
+      <c r="C1" s="127"/>
+      <c r="D1" s="127"/>
+      <c r="E1" s="83"/>
+      <c r="F1" s="83"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="127" t="s">
+        <v>202</v>
+      </c>
+      <c r="B2" s="127"/>
+      <c r="C2" s="127"/>
+      <c r="D2" s="127"/>
+      <c r="E2" s="83"/>
+      <c r="F2" s="83"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="93" t="s">
+        <v>203</v>
+      </c>
+      <c r="B4" s="93" t="s">
+        <v>204</v>
+      </c>
+      <c r="C4" s="93"/>
+      <c r="D4" s="93" t="s">
+        <v>205</v>
+      </c>
+      <c r="E4" s="93" t="s">
+        <v>205</v>
+      </c>
+      <c r="F4" s="93" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="93"/>
+      <c r="B5" s="93"/>
+      <c r="C5" s="93"/>
+      <c r="D5" s="93"/>
+      <c r="E5" s="93"/>
+      <c r="F5" s="93"/>
+    </row>
+    <row r="6" spans="1:15" ht="66.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="94" t="s">
+        <v>206</v>
+      </c>
+      <c r="B6" s="94" t="s">
+        <v>207</v>
+      </c>
+      <c r="C6" s="94" t="s">
+        <v>208</v>
+      </c>
+      <c r="D6" s="109" t="s">
+        <v>209</v>
+      </c>
+      <c r="E6" s="109" t="s">
+        <v>210</v>
+      </c>
+      <c r="F6" s="109" t="s">
+        <v>210</v>
+      </c>
+      <c r="G6" s="109" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="95">
+        <v>1</v>
+      </c>
+      <c r="B7" s="96" t="str">
+        <f>[3]Pengetahuan!B6</f>
+        <v>Adita Dwi Rezeki P</v>
+      </c>
+      <c r="C7" s="97">
+        <v>75</v>
+      </c>
+      <c r="D7" s="107">
+        <v>75</v>
+      </c>
+      <c r="E7" s="98">
+        <f>AVERAGE(C7:D7)</f>
+        <v>75</v>
+      </c>
+      <c r="F7" s="98" t="str">
+        <f>HLOOKUP(E7,$I$7:$O$9,3,TRUE)</f>
+        <v>TL</v>
+      </c>
+      <c r="G7" s="108" t="str">
+        <f>IF(E7&gt;=76,"Aman",IF(E7&lt;76,"Remed",))</f>
+        <v>Remed</v>
+      </c>
+      <c r="I7" s="81" t="s">
+        <v>232</v>
+      </c>
+      <c r="J7" s="82">
+        <v>70</v>
+      </c>
+      <c r="K7" s="82">
+        <v>76</v>
+      </c>
+      <c r="L7" s="82">
+        <v>81</v>
+      </c>
+      <c r="M7" s="82">
+        <v>86</v>
+      </c>
+      <c r="N7" s="82">
+        <v>90</v>
+      </c>
+      <c r="O7" s="82">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="95">
+        <v>2</v>
+      </c>
+      <c r="B8" s="96" t="str">
+        <f>[3]Pengetahuan!B7</f>
+        <v>Aditya Gufran</v>
+      </c>
+      <c r="C8" s="97">
+        <v>95</v>
+      </c>
+      <c r="D8" s="107">
+        <v>80</v>
+      </c>
+      <c r="E8" s="98">
+        <f t="shared" ref="E8:E28" si="0">AVERAGE(C8:D8)</f>
+        <v>87.5</v>
+      </c>
+      <c r="F8" s="98" t="str">
+        <f t="shared" ref="F8:F28" si="1">HLOOKUP(E8,$I$7:$O$9,3,TRUE)</f>
+        <v>C</v>
+      </c>
+      <c r="G8" s="108" t="str">
+        <f t="shared" ref="G8:G28" si="2">IF(E8&gt;=76,"Aman",IF(E8&lt;76,"Remed",))</f>
+        <v>Aman</v>
+      </c>
+      <c r="I8" s="81" t="s">
+        <v>231</v>
+      </c>
+      <c r="J8" s="82" t="s">
+        <v>229</v>
+      </c>
+      <c r="K8" s="82" t="s">
+        <v>218</v>
+      </c>
+      <c r="L8" s="82" t="s">
+        <v>219</v>
+      </c>
+      <c r="M8" s="82" t="s">
+        <v>220</v>
+      </c>
+      <c r="N8" s="82" t="s">
+        <v>221</v>
+      </c>
+      <c r="O8" s="82" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="95">
+        <v>3</v>
+      </c>
+      <c r="B9" s="96" t="str">
+        <f>[3]Pengetahuan!B8</f>
+        <v>Al Adlu Vitrah</v>
+      </c>
+      <c r="C9" s="97">
+        <v>95</v>
+      </c>
+      <c r="D9" s="107">
+        <v>80</v>
+      </c>
+      <c r="E9" s="98">
+        <f t="shared" si="0"/>
+        <v>87.5</v>
+      </c>
+      <c r="F9" s="98" t="str">
+        <f t="shared" si="1"/>
+        <v>C</v>
+      </c>
+      <c r="G9" s="108" t="str">
+        <f t="shared" si="2"/>
+        <v>Aman</v>
+      </c>
+      <c r="I9" s="81" t="s">
+        <v>230</v>
+      </c>
+      <c r="J9" s="82" t="s">
+        <v>226</v>
+      </c>
+      <c r="K9" s="82" t="s">
+        <v>225</v>
+      </c>
+      <c r="L9" s="82" t="s">
+        <v>224</v>
+      </c>
+      <c r="M9" s="82" t="s">
+        <v>223</v>
+      </c>
+      <c r="N9" s="82" t="s">
+        <v>212</v>
+      </c>
+      <c r="O9" s="82" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="95">
+        <v>4</v>
+      </c>
+      <c r="B10" s="96" t="str">
+        <f>[3]Pengetahuan!B9</f>
+        <v>Aulia Rahman</v>
+      </c>
+      <c r="C10" s="97">
+        <v>95</v>
+      </c>
+      <c r="D10" s="107">
+        <v>80</v>
+      </c>
+      <c r="E10" s="98">
+        <f t="shared" si="0"/>
+        <v>87.5</v>
+      </c>
+      <c r="F10" s="98" t="str">
+        <f t="shared" si="1"/>
+        <v>C</v>
+      </c>
+      <c r="G10" s="108" t="str">
+        <f t="shared" si="2"/>
+        <v>Aman</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="95">
+        <v>5</v>
+      </c>
+      <c r="B11" s="96" t="str">
+        <f>[3]Pengetahuan!B10</f>
+        <v>Bunga Azza Delia</v>
+      </c>
+      <c r="C11" s="97">
+        <v>95</v>
+      </c>
+      <c r="D11" s="107">
+        <v>80</v>
+      </c>
+      <c r="E11" s="98">
+        <f t="shared" si="0"/>
+        <v>87.5</v>
+      </c>
+      <c r="F11" s="98" t="str">
+        <f t="shared" si="1"/>
+        <v>C</v>
+      </c>
+      <c r="G11" s="108" t="str">
+        <f t="shared" si="2"/>
+        <v>Aman</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="95">
+        <v>6</v>
+      </c>
+      <c r="B12" s="96" t="str">
+        <f>[3]Pengetahuan!B11</f>
+        <v>Celci Monica</v>
+      </c>
+      <c r="C12" s="97">
+        <v>95</v>
+      </c>
+      <c r="D12" s="107">
+        <v>80</v>
+      </c>
+      <c r="E12" s="98">
+        <f t="shared" si="0"/>
+        <v>87.5</v>
+      </c>
+      <c r="F12" s="98" t="str">
+        <f t="shared" si="1"/>
+        <v>C</v>
+      </c>
+      <c r="G12" s="108" t="str">
+        <f t="shared" si="2"/>
+        <v>Aman</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="95">
+        <v>7</v>
+      </c>
+      <c r="B13" s="96" t="str">
+        <f>[3]Pengetahuan!B12</f>
+        <v>Dea Selpina</v>
+      </c>
+      <c r="C13" s="97">
+        <v>95</v>
+      </c>
+      <c r="D13" s="107">
+        <v>80</v>
+      </c>
+      <c r="E13" s="98">
+        <f t="shared" si="0"/>
+        <v>87.5</v>
+      </c>
+      <c r="F13" s="98" t="str">
+        <f t="shared" si="1"/>
+        <v>C</v>
+      </c>
+      <c r="G13" s="108" t="str">
+        <f t="shared" si="2"/>
+        <v>Aman</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="95">
+        <v>8</v>
+      </c>
+      <c r="B14" s="96" t="str">
+        <f>[3]Pengetahuan!B13</f>
+        <v>Dzamar Rahim</v>
+      </c>
+      <c r="C14" s="97">
+        <v>95</v>
+      </c>
+      <c r="D14" s="107">
+        <v>80</v>
+      </c>
+      <c r="E14" s="98">
+        <f t="shared" si="0"/>
+        <v>87.5</v>
+      </c>
+      <c r="F14" s="98" t="str">
+        <f t="shared" si="1"/>
+        <v>C</v>
+      </c>
+      <c r="G14" s="108" t="str">
+        <f t="shared" si="2"/>
+        <v>Aman</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="95">
+        <v>9</v>
+      </c>
+      <c r="B15" s="96" t="str">
+        <f>[3]Pengetahuan!B14</f>
+        <v>Indah Rahayu</v>
+      </c>
+      <c r="C15" s="97">
+        <v>95</v>
+      </c>
+      <c r="D15" s="107">
+        <v>80</v>
+      </c>
+      <c r="E15" s="98">
+        <f t="shared" si="0"/>
+        <v>87.5</v>
+      </c>
+      <c r="F15" s="98" t="str">
+        <f t="shared" si="1"/>
+        <v>C</v>
+      </c>
+      <c r="G15" s="108" t="str">
+        <f t="shared" si="2"/>
+        <v>Aman</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="95">
+        <v>10</v>
+      </c>
+      <c r="B16" s="96" t="str">
+        <f>[3]Pengetahuan!B15</f>
+        <v>Jihan Raihanah</v>
+      </c>
+      <c r="C16" s="97">
+        <v>95</v>
+      </c>
+      <c r="D16" s="107">
+        <v>80</v>
+      </c>
+      <c r="E16" s="98">
+        <f t="shared" si="0"/>
+        <v>87.5</v>
+      </c>
+      <c r="F16" s="98" t="str">
+        <f t="shared" si="1"/>
+        <v>C</v>
+      </c>
+      <c r="G16" s="108" t="str">
+        <f t="shared" si="2"/>
+        <v>Aman</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="95">
+        <v>11</v>
+      </c>
+      <c r="B17" s="96" t="str">
+        <f>[3]Pengetahuan!B16</f>
+        <v>M. Fahri</v>
+      </c>
+      <c r="C17" s="97">
+        <v>95</v>
+      </c>
+      <c r="D17" s="107">
+        <v>80</v>
+      </c>
+      <c r="E17" s="98">
+        <f t="shared" si="0"/>
+        <v>87.5</v>
+      </c>
+      <c r="F17" s="98" t="str">
+        <f t="shared" si="1"/>
+        <v>C</v>
+      </c>
+      <c r="G17" s="108" t="str">
+        <f t="shared" si="2"/>
+        <v>Aman</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="95">
+        <v>12</v>
+      </c>
+      <c r="B18" s="96" t="str">
+        <f>[3]Pengetahuan!B17</f>
+        <v>M. Rifki</v>
+      </c>
+      <c r="C18" s="97">
+        <v>95</v>
+      </c>
+      <c r="D18" s="107">
+        <v>80</v>
+      </c>
+      <c r="E18" s="98">
+        <f t="shared" si="0"/>
+        <v>87.5</v>
+      </c>
+      <c r="F18" s="98" t="str">
+        <f t="shared" si="1"/>
+        <v>C</v>
+      </c>
+      <c r="G18" s="108" t="str">
+        <f t="shared" si="2"/>
+        <v>Aman</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="95">
+        <v>13</v>
+      </c>
+      <c r="B19" s="96" t="str">
+        <f>[3]Pengetahuan!B18</f>
+        <v>M. Sulthan Khair</v>
+      </c>
+      <c r="C19" s="97">
+        <v>95</v>
+      </c>
+      <c r="D19" s="107">
+        <v>80</v>
+      </c>
+      <c r="E19" s="98">
+        <f t="shared" si="0"/>
+        <v>87.5</v>
+      </c>
+      <c r="F19" s="98" t="str">
+        <f t="shared" si="1"/>
+        <v>C</v>
+      </c>
+      <c r="G19" s="108" t="str">
+        <f t="shared" si="2"/>
+        <v>Aman</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="95">
+        <v>14</v>
+      </c>
+      <c r="B20" s="96" t="str">
+        <f>[3]Pengetahuan!B19</f>
+        <v>Nabila Putri</v>
+      </c>
+      <c r="C20" s="97">
+        <v>95</v>
+      </c>
+      <c r="D20" s="107">
+        <v>80</v>
+      </c>
+      <c r="E20" s="98">
+        <f t="shared" si="0"/>
+        <v>87.5</v>
+      </c>
+      <c r="F20" s="98" t="str">
+        <f t="shared" si="1"/>
+        <v>C</v>
+      </c>
+      <c r="G20" s="108" t="str">
+        <f t="shared" si="2"/>
+        <v>Aman</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="95">
+        <v>15</v>
+      </c>
+      <c r="B21" s="96" t="str">
+        <f>[3]Pengetahuan!B20</f>
+        <v>Putri Amelia</v>
+      </c>
+      <c r="C21" s="97">
+        <v>95</v>
+      </c>
+      <c r="D21" s="107">
+        <v>80</v>
+      </c>
+      <c r="E21" s="98">
+        <f t="shared" si="0"/>
+        <v>87.5</v>
+      </c>
+      <c r="F21" s="98" t="str">
+        <f t="shared" si="1"/>
+        <v>C</v>
+      </c>
+      <c r="G21" s="108" t="str">
+        <f t="shared" si="2"/>
+        <v>Aman</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="95">
+        <v>16</v>
+      </c>
+      <c r="B22" s="96" t="str">
+        <f>[3]Pengetahuan!B21</f>
+        <v>Rina Ramadani</v>
+      </c>
+      <c r="C22" s="97">
+        <v>95</v>
+      </c>
+      <c r="D22" s="107">
+        <v>80</v>
+      </c>
+      <c r="E22" s="98">
+        <f t="shared" si="0"/>
+        <v>87.5</v>
+      </c>
+      <c r="F22" s="98" t="str">
+        <f t="shared" si="1"/>
+        <v>C</v>
+      </c>
+      <c r="G22" s="108" t="str">
+        <f t="shared" si="2"/>
+        <v>Aman</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="95">
+        <v>17</v>
+      </c>
+      <c r="B23" s="96" t="str">
+        <f>[3]Pengetahuan!B22</f>
+        <v>Ryan Fahlevi</v>
+      </c>
+      <c r="C23" s="97">
+        <v>95</v>
+      </c>
+      <c r="D23" s="107">
+        <v>80</v>
+      </c>
+      <c r="E23" s="98">
+        <f t="shared" si="0"/>
+        <v>87.5</v>
+      </c>
+      <c r="F23" s="98" t="str">
+        <f t="shared" si="1"/>
+        <v>C</v>
+      </c>
+      <c r="G23" s="108" t="str">
+        <f t="shared" si="2"/>
+        <v>Aman</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="95">
+        <v>18</v>
+      </c>
+      <c r="B24" s="96" t="str">
+        <f>[3]Pengetahuan!B23</f>
+        <v>Sherly Amanda Elysia</v>
+      </c>
+      <c r="C24" s="97">
+        <v>95</v>
+      </c>
+      <c r="D24" s="107">
+        <v>80</v>
+      </c>
+      <c r="E24" s="98">
+        <f t="shared" si="0"/>
+        <v>87.5</v>
+      </c>
+      <c r="F24" s="98" t="str">
+        <f t="shared" si="1"/>
+        <v>C</v>
+      </c>
+      <c r="G24" s="108" t="str">
+        <f t="shared" si="2"/>
+        <v>Aman</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="95">
+        <v>19</v>
+      </c>
+      <c r="B25" s="96" t="str">
+        <f>[3]Pengetahuan!B24</f>
+        <v>Sri Ariyani</v>
+      </c>
+      <c r="C25" s="97">
+        <v>95</v>
+      </c>
+      <c r="D25" s="107">
+        <v>80</v>
+      </c>
+      <c r="E25" s="98">
+        <f t="shared" si="0"/>
+        <v>87.5</v>
+      </c>
+      <c r="F25" s="98" t="str">
+        <f t="shared" si="1"/>
+        <v>C</v>
+      </c>
+      <c r="G25" s="108" t="str">
+        <f t="shared" si="2"/>
+        <v>Aman</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="95">
+        <v>20</v>
+      </c>
+      <c r="B26" s="96" t="str">
+        <f>[3]Pengetahuan!B25</f>
+        <v>T. Amylia Safitri</v>
+      </c>
+      <c r="C26" s="97">
+        <v>95</v>
+      </c>
+      <c r="D26" s="107">
+        <v>80</v>
+      </c>
+      <c r="E26" s="98">
+        <f t="shared" si="0"/>
+        <v>87.5</v>
+      </c>
+      <c r="F26" s="98" t="str">
+        <f t="shared" si="1"/>
+        <v>C</v>
+      </c>
+      <c r="G26" s="108" t="str">
+        <f t="shared" si="2"/>
+        <v>Aman</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="95">
+        <v>21</v>
+      </c>
+      <c r="B27" s="96" t="str">
+        <f>[3]Pengetahuan!B26</f>
+        <v>Windi Safira</v>
+      </c>
+      <c r="C27" s="97">
+        <v>95</v>
+      </c>
+      <c r="D27" s="107">
+        <v>80</v>
+      </c>
+      <c r="E27" s="98">
+        <f t="shared" si="0"/>
+        <v>87.5</v>
+      </c>
+      <c r="F27" s="98" t="str">
+        <f t="shared" si="1"/>
+        <v>C</v>
+      </c>
+      <c r="G27" s="108" t="str">
+        <f t="shared" si="2"/>
+        <v>Aman</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="95">
+        <v>22</v>
+      </c>
+      <c r="B28" s="96" t="str">
+        <f>[3]Pengetahuan!B27</f>
+        <v>Zahwa Maila Puspita</v>
+      </c>
+      <c r="C28" s="97">
+        <v>95</v>
+      </c>
+      <c r="D28" s="107">
+        <v>80</v>
+      </c>
+      <c r="E28" s="98">
+        <f t="shared" si="0"/>
+        <v>87.5</v>
+      </c>
+      <c r="F28" s="98" t="str">
+        <f t="shared" si="1"/>
+        <v>C</v>
+      </c>
+      <c r="G28" s="108" t="str">
+        <f t="shared" si="2"/>
+        <v>Aman</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="99"/>
+      <c r="B29" s="100"/>
+      <c r="C29" s="101"/>
+      <c r="D29" s="101"/>
+      <c r="E29" s="101"/>
+      <c r="F29" s="101"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="99"/>
+      <c r="B30" s="100"/>
+      <c r="C30" s="101"/>
+      <c r="D30" s="101"/>
+      <c r="E30" s="101"/>
+      <c r="F30" s="101"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="102"/>
+      <c r="B31" s="102" t="s">
+        <v>213</v>
+      </c>
+      <c r="C31" s="103">
+        <f>AVERAGE(C7:C30)</f>
+        <v>94.090909090909093</v>
+      </c>
+      <c r="D31" s="103">
+        <f>AVERAGE(D7:D30)</f>
+        <v>79.772727272727266</v>
+      </c>
+      <c r="E31" s="103">
+        <f>AVERAGE(E7:E30)</f>
+        <v>86.931818181818187</v>
+      </c>
+      <c r="F31" s="103" t="e">
+        <f>AVERAGE(F7:F30)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G31" s="104">
+        <f>COUNTIF(G7:G28,"Remed")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="99"/>
+      <c r="B32" s="99"/>
+      <c r="C32" s="101"/>
+      <c r="D32" s="101"/>
+      <c r="E32" s="101"/>
+      <c r="F32" s="101"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="93"/>
+      <c r="B33" s="93"/>
+      <c r="C33" s="93" t="s">
+        <v>214</v>
+      </c>
+      <c r="D33" s="93"/>
+      <c r="E33" s="93"/>
+      <c r="F33" s="93"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="93"/>
+      <c r="B34" s="93"/>
+      <c r="C34" s="93" t="s">
+        <v>215</v>
+      </c>
+      <c r="D34" s="93" t="s">
+        <v>216</v>
+      </c>
+      <c r="E34" s="93" t="s">
+        <v>216</v>
+      </c>
+      <c r="F34" s="93" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="93"/>
+      <c r="B35" s="93"/>
+      <c r="C35" s="93"/>
+      <c r="D35" s="93"/>
+      <c r="E35" s="93"/>
+      <c r="F35" s="93"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="93"/>
+      <c r="B36" s="93"/>
+      <c r="C36" s="93"/>
+      <c r="D36" s="93"/>
+      <c r="E36" s="93"/>
+      <c r="F36" s="93"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="93"/>
+      <c r="B37" s="93"/>
+      <c r="C37" s="128" t="s">
+        <v>155</v>
+      </c>
+      <c r="D37" s="128"/>
+      <c r="E37" s="105"/>
+      <c r="F37" s="105"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="93"/>
+      <c r="B38" s="93"/>
+      <c r="C38" s="129" t="s">
+        <v>217</v>
+      </c>
+      <c r="D38" s="129"/>
+      <c r="E38" s="106"/>
+      <c r="F38" s="106"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C38:D38"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -3611,7 +5715,7 @@
   <dimension ref="A1:AG20"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -3623,86 +5727,86 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" s="39" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="83" t="s">
+      <c r="A1" s="112" t="s">
         <v>151</v>
       </c>
-      <c r="B1" s="83"/>
-      <c r="C1" s="83"/>
-      <c r="D1" s="83"/>
-      <c r="E1" s="83"/>
-      <c r="F1" s="83"/>
-      <c r="G1" s="83"/>
-      <c r="H1" s="83"/>
-      <c r="I1" s="83"/>
-      <c r="J1" s="83"/>
-      <c r="K1" s="83"/>
-      <c r="L1" s="83"/>
-      <c r="M1" s="83"/>
-      <c r="N1" s="83"/>
-      <c r="O1" s="83"/>
-      <c r="P1" s="83"/>
-      <c r="Q1" s="83"/>
-      <c r="R1" s="83"/>
-      <c r="S1" s="83"/>
-      <c r="T1" s="83"/>
-      <c r="U1" s="83"/>
-      <c r="V1" s="83"/>
-      <c r="W1" s="83"/>
-      <c r="X1" s="83"/>
-      <c r="Y1" s="83"/>
-      <c r="Z1" s="83"/>
-      <c r="AA1" s="83"/>
-      <c r="AB1" s="83"/>
-      <c r="AC1" s="83"/>
-      <c r="AD1" s="83"/>
-      <c r="AE1" s="83"/>
-      <c r="AF1" s="83"/>
-      <c r="AG1" s="83"/>
+      <c r="B1" s="112"/>
+      <c r="C1" s="112"/>
+      <c r="D1" s="112"/>
+      <c r="E1" s="112"/>
+      <c r="F1" s="112"/>
+      <c r="G1" s="112"/>
+      <c r="H1" s="112"/>
+      <c r="I1" s="112"/>
+      <c r="J1" s="112"/>
+      <c r="K1" s="112"/>
+      <c r="L1" s="112"/>
+      <c r="M1" s="112"/>
+      <c r="N1" s="112"/>
+      <c r="O1" s="112"/>
+      <c r="P1" s="112"/>
+      <c r="Q1" s="112"/>
+      <c r="R1" s="112"/>
+      <c r="S1" s="112"/>
+      <c r="T1" s="112"/>
+      <c r="U1" s="112"/>
+      <c r="V1" s="112"/>
+      <c r="W1" s="112"/>
+      <c r="X1" s="112"/>
+      <c r="Y1" s="112"/>
+      <c r="Z1" s="112"/>
+      <c r="AA1" s="112"/>
+      <c r="AB1" s="112"/>
+      <c r="AC1" s="112"/>
+      <c r="AD1" s="112"/>
+      <c r="AE1" s="112"/>
+      <c r="AF1" s="112"/>
+      <c r="AG1" s="112"/>
     </row>
     <row r="3" spans="1:33" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="84" t="s">
+      <c r="A3" s="113" t="s">
         <v>67</v>
       </c>
-      <c r="B3" s="85" t="s">
+      <c r="B3" s="114" t="s">
         <v>68</v>
       </c>
-      <c r="C3" s="86" t="s">
+      <c r="C3" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="D3" s="86"/>
-      <c r="E3" s="86"/>
-      <c r="F3" s="86"/>
-      <c r="G3" s="86"/>
-      <c r="H3" s="86"/>
-      <c r="I3" s="86"/>
-      <c r="J3" s="86"/>
-      <c r="K3" s="86"/>
-      <c r="L3" s="86"/>
-      <c r="M3" s="86"/>
-      <c r="N3" s="86"/>
-      <c r="O3" s="86"/>
-      <c r="P3" s="86"/>
-      <c r="Q3" s="86"/>
-      <c r="R3" s="86"/>
-      <c r="S3" s="86"/>
-      <c r="T3" s="86"/>
-      <c r="U3" s="86"/>
-      <c r="V3" s="86"/>
-      <c r="W3" s="86"/>
-      <c r="X3" s="86"/>
-      <c r="Y3" s="86"/>
-      <c r="Z3" s="86"/>
-      <c r="AA3" s="86"/>
-      <c r="AB3" s="86"/>
-      <c r="AC3" s="86"/>
-      <c r="AD3" s="86"/>
-      <c r="AE3" s="86"/>
-      <c r="AF3" s="86"/>
-      <c r="AG3" s="86"/>
+      <c r="D3" s="115"/>
+      <c r="E3" s="115"/>
+      <c r="F3" s="115"/>
+      <c r="G3" s="115"/>
+      <c r="H3" s="115"/>
+      <c r="I3" s="115"/>
+      <c r="J3" s="115"/>
+      <c r="K3" s="115"/>
+      <c r="L3" s="115"/>
+      <c r="M3" s="115"/>
+      <c r="N3" s="115"/>
+      <c r="O3" s="115"/>
+      <c r="P3" s="115"/>
+      <c r="Q3" s="115"/>
+      <c r="R3" s="115"/>
+      <c r="S3" s="115"/>
+      <c r="T3" s="115"/>
+      <c r="U3" s="115"/>
+      <c r="V3" s="115"/>
+      <c r="W3" s="115"/>
+      <c r="X3" s="115"/>
+      <c r="Y3" s="115"/>
+      <c r="Z3" s="115"/>
+      <c r="AA3" s="115"/>
+      <c r="AB3" s="115"/>
+      <c r="AC3" s="115"/>
+      <c r="AD3" s="115"/>
+      <c r="AE3" s="115"/>
+      <c r="AF3" s="115"/>
+      <c r="AG3" s="115"/>
     </row>
     <row r="4" spans="1:33" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="84"/>
-      <c r="B4" s="85"/>
+      <c r="A4" s="113"/>
+      <c r="B4" s="114"/>
       <c r="C4" s="41">
         <v>1</v>
       </c>
@@ -3786,8 +5890,8 @@
       </c>
     </row>
     <row r="5" spans="1:33" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="84"/>
-      <c r="B5" s="85"/>
+      <c r="A5" s="113"/>
+      <c r="B5" s="114"/>
       <c r="C5" s="42">
         <v>20</v>
       </c>
@@ -3883,8 +5987,8 @@
       </c>
     </row>
     <row r="6" spans="1:33" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="84"/>
-      <c r="B6" s="85"/>
+      <c r="A6" s="113"/>
+      <c r="B6" s="114"/>
       <c r="C6" s="44" t="s">
         <v>70</v>
       </c>
@@ -4509,9 +6613,7 @@
       <c r="A19" s="48" t="s">
         <v>88</v>
       </c>
-      <c r="B19" s="49">
-        <v>10</v>
-      </c>
+      <c r="B19" s="49"/>
       <c r="C19" s="42"/>
       <c r="D19" s="42"/>
       <c r="E19" s="42"/>
@@ -4552,37 +6654,37 @@
         <f>SUM(B8:B18)</f>
         <v>201</v>
       </c>
-      <c r="C20" s="87"/>
-      <c r="D20" s="88"/>
-      <c r="E20" s="88"/>
-      <c r="F20" s="88"/>
-      <c r="G20" s="88"/>
-      <c r="H20" s="88"/>
-      <c r="I20" s="88"/>
-      <c r="J20" s="88"/>
-      <c r="K20" s="88"/>
-      <c r="L20" s="88"/>
-      <c r="M20" s="88"/>
-      <c r="N20" s="88"/>
-      <c r="O20" s="88"/>
-      <c r="P20" s="88"/>
-      <c r="Q20" s="88"/>
-      <c r="R20" s="88"/>
-      <c r="S20" s="88"/>
-      <c r="T20" s="88"/>
-      <c r="U20" s="88"/>
-      <c r="V20" s="88"/>
-      <c r="W20" s="88"/>
-      <c r="X20" s="88"/>
-      <c r="Y20" s="88"/>
-      <c r="Z20" s="88"/>
-      <c r="AA20" s="88"/>
-      <c r="AB20" s="88"/>
-      <c r="AC20" s="88"/>
-      <c r="AD20" s="88"/>
-      <c r="AE20" s="88"/>
-      <c r="AF20" s="88"/>
-      <c r="AG20" s="88"/>
+      <c r="C20" s="116"/>
+      <c r="D20" s="117"/>
+      <c r="E20" s="117"/>
+      <c r="F20" s="117"/>
+      <c r="G20" s="117"/>
+      <c r="H20" s="117"/>
+      <c r="I20" s="117"/>
+      <c r="J20" s="117"/>
+      <c r="K20" s="117"/>
+      <c r="L20" s="117"/>
+      <c r="M20" s="117"/>
+      <c r="N20" s="117"/>
+      <c r="O20" s="117"/>
+      <c r="P20" s="117"/>
+      <c r="Q20" s="117"/>
+      <c r="R20" s="117"/>
+      <c r="S20" s="117"/>
+      <c r="T20" s="117"/>
+      <c r="U20" s="117"/>
+      <c r="V20" s="117"/>
+      <c r="W20" s="117"/>
+      <c r="X20" s="117"/>
+      <c r="Y20" s="117"/>
+      <c r="Z20" s="117"/>
+      <c r="AA20" s="117"/>
+      <c r="AB20" s="117"/>
+      <c r="AC20" s="117"/>
+      <c r="AD20" s="117"/>
+      <c r="AE20" s="117"/>
+      <c r="AF20" s="117"/>
+      <c r="AG20" s="117"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -4599,10 +6701,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="1"/>
+  </sheetPr>
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20:B21"/>
+    <sheetView view="pageBreakPreview" topLeftCell="B1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4618,28 +6723,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="89" t="s">
+      <c r="A1" s="118" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="89"/>
-      <c r="C1" s="89"/>
-      <c r="D1" s="89"/>
-      <c r="E1" s="89"/>
-      <c r="F1" s="89"/>
-      <c r="G1" s="89"/>
-      <c r="H1" s="89"/>
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
+      <c r="D1" s="118"/>
+      <c r="E1" s="118"/>
+      <c r="F1" s="118"/>
+      <c r="G1" s="118"/>
+      <c r="H1" s="118"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="89" t="s">
+      <c r="A2" s="118" t="s">
         <v>97</v>
       </c>
-      <c r="B2" s="89"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="89"/>
-      <c r="H2" s="89"/>
+      <c r="B2" s="118"/>
+      <c r="C2" s="118"/>
+      <c r="D2" s="118"/>
+      <c r="E2" s="118"/>
+      <c r="F2" s="118"/>
+      <c r="G2" s="118"/>
+      <c r="H2" s="118"/>
     </row>
     <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="56"/>
@@ -4681,14 +6786,14 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="90"/>
-      <c r="B6" s="91"/>
-      <c r="C6" s="91"/>
-      <c r="D6" s="91"/>
-      <c r="E6" s="91"/>
-      <c r="F6" s="91"/>
-      <c r="G6" s="91"/>
-      <c r="H6" s="92"/>
+      <c r="A6" s="119"/>
+      <c r="B6" s="120"/>
+      <c r="C6" s="120"/>
+      <c r="D6" s="120"/>
+      <c r="E6" s="120"/>
+      <c r="F6" s="120"/>
+      <c r="G6" s="120"/>
+      <c r="H6" s="121"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="62">
@@ -5096,10 +7201,10 @@
       </c>
     </row>
     <row r="22" spans="1:8" s="68" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="93" t="s">
+      <c r="A22" s="122" t="s">
         <v>8</v>
       </c>
-      <c r="B22" s="94"/>
+      <c r="B22" s="123"/>
       <c r="C22" s="66"/>
       <c r="D22" s="66"/>
       <c r="E22" s="66"/>
@@ -5178,10 +7283,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:G18"/>
+  <dimension ref="A3:J21"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="H3" sqref="H3:J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5192,7 +7297,7 @@
     <col min="4" max="4" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="53" t="s">
         <v>4</v>
       </c>
@@ -5211,9 +7316,18 @@
       <c r="F3" s="53" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="96">
+      <c r="H3" s="81" t="s">
+        <v>165</v>
+      </c>
+      <c r="I3" s="81" t="s">
+        <v>171</v>
+      </c>
+      <c r="J3" s="81" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="82">
         <v>1</v>
       </c>
       <c r="B4" s="38" t="s">
@@ -5223,20 +7337,29 @@
         <v>5000</v>
       </c>
       <c r="D4" s="54">
-        <f>C4+1000</f>
+        <f t="shared" ref="D4:F13" si="0">C4+1000</f>
         <v>6000</v>
       </c>
       <c r="E4" s="54">
-        <f>D4+1000</f>
+        <f t="shared" si="0"/>
         <v>7000</v>
       </c>
       <c r="F4" s="54">
-        <f>E4+1000</f>
+        <f t="shared" si="0"/>
         <v>8000</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="96">
+      <c r="H4" s="38" t="s">
+        <v>159</v>
+      </c>
+      <c r="I4" s="38" t="s">
+        <v>166</v>
+      </c>
+      <c r="J4" s="38" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="82">
         <v>2</v>
       </c>
       <c r="B5" s="38" t="s">
@@ -5246,20 +7369,29 @@
         <v>5000</v>
       </c>
       <c r="D5" s="54">
-        <f>C5+1000</f>
+        <f t="shared" si="0"/>
         <v>6000</v>
       </c>
       <c r="E5" s="54">
-        <f>D5+1000</f>
+        <f t="shared" si="0"/>
         <v>7000</v>
       </c>
       <c r="F5" s="54">
-        <f>E5+1000</f>
+        <f t="shared" si="0"/>
         <v>8000</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="96">
+      <c r="H5" s="38" t="s">
+        <v>160</v>
+      </c>
+      <c r="I5" s="38" t="s">
+        <v>166</v>
+      </c>
+      <c r="J5" s="38" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="82">
         <v>3</v>
       </c>
       <c r="B6" s="38" t="s">
@@ -5269,20 +7401,29 @@
         <v>13000</v>
       </c>
       <c r="D6" s="54">
-        <f>C6+1000</f>
+        <f t="shared" si="0"/>
         <v>14000</v>
       </c>
       <c r="E6" s="54">
-        <f>D6+1000</f>
+        <f t="shared" si="0"/>
         <v>15000</v>
       </c>
       <c r="F6" s="54">
-        <f>E6+1000</f>
+        <f t="shared" si="0"/>
         <v>16000</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="96">
+      <c r="H6" s="38" t="s">
+        <v>161</v>
+      </c>
+      <c r="I6" s="38" t="s">
+        <v>167</v>
+      </c>
+      <c r="J6" s="38" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="82">
         <v>4</v>
       </c>
       <c r="B7" s="38" t="s">
@@ -5292,20 +7433,29 @@
         <v>15000</v>
       </c>
       <c r="D7" s="54">
-        <f>C7+1000</f>
+        <f t="shared" si="0"/>
         <v>16000</v>
       </c>
       <c r="E7" s="54">
-        <f>D7+1000</f>
+        <f t="shared" si="0"/>
         <v>17000</v>
       </c>
       <c r="F7" s="54">
-        <f>E7+1000</f>
+        <f t="shared" si="0"/>
         <v>18000</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="96">
+      <c r="H7" s="38" t="s">
+        <v>162</v>
+      </c>
+      <c r="I7" s="38" t="s">
+        <v>168</v>
+      </c>
+      <c r="J7" s="38" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="82">
         <v>5</v>
       </c>
       <c r="B8" s="38" t="s">
@@ -5315,20 +7465,29 @@
         <v>5000</v>
       </c>
       <c r="D8" s="54">
-        <f>C8+1000</f>
+        <f t="shared" si="0"/>
         <v>6000</v>
       </c>
       <c r="E8" s="54">
-        <f>D8+1000</f>
+        <f t="shared" si="0"/>
         <v>7000</v>
       </c>
       <c r="F8" s="54">
-        <f>E8+1000</f>
+        <f t="shared" si="0"/>
         <v>8000</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="96">
+      <c r="H8" s="38" t="s">
+        <v>163</v>
+      </c>
+      <c r="I8" s="38" t="s">
+        <v>169</v>
+      </c>
+      <c r="J8" s="38" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="82">
         <v>6</v>
       </c>
       <c r="B9" s="38" t="s">
@@ -5338,20 +7497,29 @@
         <v>10000</v>
       </c>
       <c r="D9" s="54">
-        <f>C9+1000</f>
+        <f t="shared" si="0"/>
         <v>11000</v>
       </c>
       <c r="E9" s="54">
-        <f>D9+1000</f>
+        <f t="shared" si="0"/>
         <v>12000</v>
       </c>
       <c r="F9" s="54">
-        <f>E9+1000</f>
+        <f t="shared" si="0"/>
         <v>13000</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="96">
+      <c r="H9" s="38" t="s">
+        <v>164</v>
+      </c>
+      <c r="I9" s="38" t="s">
+        <v>170</v>
+      </c>
+      <c r="J9" s="38" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="82">
         <v>7</v>
       </c>
       <c r="B10" s="38" t="s">
@@ -5361,20 +7529,20 @@
         <v>40000</v>
       </c>
       <c r="D10" s="54">
-        <f>C10+1000</f>
+        <f t="shared" si="0"/>
         <v>41000</v>
       </c>
       <c r="E10" s="54">
-        <f>D10+1000</f>
+        <f t="shared" si="0"/>
         <v>42000</v>
       </c>
       <c r="F10" s="54">
-        <f>E10+1000</f>
+        <f t="shared" si="0"/>
         <v>43000</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="96">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="82">
         <v>8</v>
       </c>
       <c r="B11" s="38" t="s">
@@ -5384,68 +7552,79 @@
         <v>200000</v>
       </c>
       <c r="D11" s="54">
-        <f>C11+1000</f>
+        <f t="shared" si="0"/>
         <v>201000</v>
       </c>
       <c r="E11" s="54">
-        <f>D11+1000</f>
+        <f t="shared" si="0"/>
         <v>202000</v>
       </c>
       <c r="F11" s="54">
-        <f>E11+1000</f>
+        <f t="shared" si="0"/>
         <v>203000</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="104">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="90">
         <v>9</v>
       </c>
-      <c r="B12" s="103" t="s">
+      <c r="B12" s="89" t="s">
         <v>157</v>
       </c>
-      <c r="C12" s="105">
+      <c r="C12" s="91">
         <v>100000</v>
       </c>
-      <c r="D12" s="105">
-        <f>C12+1000</f>
+      <c r="D12" s="91">
+        <f t="shared" si="0"/>
         <v>101000</v>
       </c>
-      <c r="E12" s="105">
-        <f>D12+1000</f>
+      <c r="E12" s="91">
+        <f t="shared" si="0"/>
         <v>102000</v>
       </c>
-      <c r="F12" s="105">
-        <f>E12+1000</f>
+      <c r="F12" s="91">
+        <f t="shared" si="0"/>
         <v>103000</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="104">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="90">
         <v>10</v>
       </c>
-      <c r="B13" s="103" t="s">
+      <c r="B13" s="89" t="s">
         <v>158</v>
       </c>
-      <c r="C13" s="105">
+      <c r="C13" s="91">
         <v>500000</v>
       </c>
-      <c r="D13" s="105">
-        <f>C13+1000</f>
+      <c r="D13" s="91">
+        <f t="shared" si="0"/>
         <v>501000</v>
       </c>
-      <c r="E13" s="105">
-        <f>D13+1000</f>
+      <c r="E13" s="91">
+        <f t="shared" si="0"/>
         <v>502000</v>
       </c>
-      <c r="F13" s="105">
-        <f>E13+1000</f>
+      <c r="F13" s="91">
+        <f t="shared" si="0"/>
         <v>503000</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="95" t="s">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="125" t="s">
+        <v>199</v>
+      </c>
+      <c r="B15" s="124" t="s">
         <v>165</v>
       </c>
+      <c r="C15" s="124"/>
+      <c r="D15" s="124"/>
+      <c r="E15" s="124"/>
+      <c r="F15" s="124"/>
+      <c r="G15" s="124"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="126"/>
       <c r="B16" s="38" t="s">
         <v>159</v>
       </c>
@@ -5466,7 +7645,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="95" t="s">
+      <c r="A17" s="81" t="s">
         <v>171</v>
       </c>
       <c r="B17" s="38" t="s">
@@ -5489,7 +7668,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="95" t="s">
+      <c r="A18" s="81" t="s">
         <v>172</v>
       </c>
       <c r="B18" s="38" t="s">
@@ -5511,7 +7690,57 @@
         <v>176</v>
       </c>
     </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="81" t="s">
+        <v>165</v>
+      </c>
+      <c r="B20" s="38" t="s">
+        <v>159</v>
+      </c>
+      <c r="C20" s="38" t="s">
+        <v>160</v>
+      </c>
+      <c r="D20" s="38" t="s">
+        <v>161</v>
+      </c>
+      <c r="E20" s="38" t="s">
+        <v>162</v>
+      </c>
+      <c r="F20" s="38" t="s">
+        <v>163</v>
+      </c>
+      <c r="G20" s="38" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="81" t="s">
+        <v>200</v>
+      </c>
+      <c r="B21" s="38" t="s">
+        <v>166</v>
+      </c>
+      <c r="C21" s="38" t="s">
+        <v>166</v>
+      </c>
+      <c r="D21" s="38" t="s">
+        <v>167</v>
+      </c>
+      <c r="E21" s="38" t="s">
+        <v>168</v>
+      </c>
+      <c r="F21" s="38" t="s">
+        <v>169</v>
+      </c>
+      <c r="G21" s="38" t="s">
+        <v>170</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="A15:A16"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -5534,32 +7763,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="97" t="s">
+      <c r="A1" s="127" t="s">
         <v>153</v>
       </c>
-      <c r="B1" s="97"/>
-      <c r="C1" s="97"/>
-      <c r="D1" s="97"/>
-      <c r="E1" s="97"/>
-      <c r="F1" s="97"/>
+      <c r="B1" s="127"/>
+      <c r="C1" s="127"/>
+      <c r="D1" s="127"/>
+      <c r="E1" s="127"/>
+      <c r="F1" s="127"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="95" t="s">
+      <c r="A3" s="81" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="95" t="s">
+      <c r="B3" s="81" t="s">
         <v>91</v>
       </c>
-      <c r="C3" s="95" t="s">
+      <c r="C3" s="81" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="95" t="s">
+      <c r="D3" s="81" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="95" t="s">
+      <c r="E3" s="81" t="s">
         <v>59</v>
       </c>
-      <c r="F3" s="95" t="s">
+      <c r="F3" s="81" t="s">
         <v>11</v>
       </c>
     </row>
@@ -5581,7 +7810,7 @@
         <v>6000</v>
       </c>
       <c r="F4" s="54">
-        <f>E4*C4</f>
+        <f t="shared" ref="F4:F11" si="0">E4*C4</f>
         <v>150000</v>
       </c>
     </row>
@@ -5603,7 +7832,7 @@
         <v>6000</v>
       </c>
       <c r="F5" s="54">
-        <f>E5*C5</f>
+        <f t="shared" si="0"/>
         <v>150000</v>
       </c>
     </row>
@@ -5625,7 +7854,7 @@
         <v>6000</v>
       </c>
       <c r="F6" s="54">
-        <f>E6*C6</f>
+        <f t="shared" si="0"/>
         <v>150000</v>
       </c>
     </row>
@@ -5647,7 +7876,7 @@
         <v>16000</v>
       </c>
       <c r="F7" s="54">
-        <f>E7*C7</f>
+        <f t="shared" si="0"/>
         <v>208000</v>
       </c>
     </row>
@@ -5669,7 +7898,7 @@
         <v>6000</v>
       </c>
       <c r="F8" s="54">
-        <f>E8*C8</f>
+        <f t="shared" si="0"/>
         <v>18000</v>
       </c>
     </row>
@@ -5691,7 +7920,7 @@
         <v>11000</v>
       </c>
       <c r="F9" s="54">
-        <f>E9*C9</f>
+        <f t="shared" si="0"/>
         <v>88000</v>
       </c>
     </row>
@@ -5713,7 +7942,7 @@
         <v>41000</v>
       </c>
       <c r="F10" s="54">
-        <f>E10*C10</f>
+        <f t="shared" si="0"/>
         <v>1025000</v>
       </c>
     </row>
@@ -5735,7 +7964,7 @@
         <v>16000</v>
       </c>
       <c r="F11" s="54">
-        <f>E11*C11</f>
+        <f t="shared" si="0"/>
         <v>16000</v>
       </c>
     </row>
@@ -5753,12 +7982,12 @@
       </c>
     </row>
     <row r="18" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E18" s="98" t="s">
+      <c r="E18" s="84" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="19" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E19" s="99" t="s">
+      <c r="E19" s="85" t="s">
         <v>156</v>
       </c>
     </row>
@@ -5788,32 +8017,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="97" t="s">
+      <c r="A1" s="127" t="s">
         <v>153</v>
       </c>
-      <c r="B1" s="97"/>
-      <c r="C1" s="97"/>
-      <c r="D1" s="97"/>
-      <c r="E1" s="97"/>
-      <c r="F1" s="97"/>
+      <c r="B1" s="127"/>
+      <c r="C1" s="127"/>
+      <c r="D1" s="127"/>
+      <c r="E1" s="127"/>
+      <c r="F1" s="127"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="95" t="s">
+      <c r="A3" s="81" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="95" t="s">
+      <c r="B3" s="81" t="s">
         <v>91</v>
       </c>
-      <c r="C3" s="95" t="s">
+      <c r="C3" s="81" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="95" t="s">
+      <c r="D3" s="81" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="95" t="s">
+      <c r="E3" s="81" t="s">
         <v>59</v>
       </c>
-      <c r="F3" s="95" t="s">
+      <c r="F3" s="81" t="s">
         <v>11</v>
       </c>
     </row>
@@ -5835,7 +8064,7 @@
         <v>5000</v>
       </c>
       <c r="F4" s="54">
-        <f>E4*C4</f>
+        <f t="shared" ref="F4:F9" si="0">E4*C4</f>
         <v>125000</v>
       </c>
     </row>
@@ -5857,7 +8086,7 @@
         <v>5000</v>
       </c>
       <c r="F5" s="54">
-        <f>E5*C5</f>
+        <f t="shared" si="0"/>
         <v>125000</v>
       </c>
     </row>
@@ -5879,7 +8108,7 @@
         <v>15000</v>
       </c>
       <c r="F6" s="54">
-        <f>E6*C6</f>
+        <f t="shared" si="0"/>
         <v>195000</v>
       </c>
     </row>
@@ -5901,7 +8130,7 @@
         <v>5000</v>
       </c>
       <c r="F7" s="54">
-        <f>E7*C7</f>
+        <f t="shared" si="0"/>
         <v>15000</v>
       </c>
     </row>
@@ -5923,7 +8152,7 @@
         <v>10000</v>
       </c>
       <c r="F8" s="54">
-        <f>E8*C8</f>
+        <f t="shared" si="0"/>
         <v>80000</v>
       </c>
     </row>
@@ -5945,7 +8174,7 @@
         <v>15000</v>
       </c>
       <c r="F9" s="54">
-        <f>E9*C9</f>
+        <f t="shared" si="0"/>
         <v>15000</v>
       </c>
     </row>
@@ -5953,7 +8182,7 @@
       <c r="A10" s="38">
         <v>7</v>
       </c>
-      <c r="B10" s="103" t="s">
+      <c r="B10" s="89" t="s">
         <v>157</v>
       </c>
       <c r="C10" s="38">
@@ -5967,7 +8196,7 @@
         <v>200000</v>
       </c>
       <c r="F10" s="54">
-        <f t="shared" ref="F10:F11" si="0">E10*C10</f>
+        <f t="shared" ref="F10:F11" si="1">E10*C10</f>
         <v>200000</v>
       </c>
     </row>
@@ -5975,7 +8204,7 @@
       <c r="A11" s="38">
         <v>8</v>
       </c>
-      <c r="B11" s="103" t="s">
+      <c r="B11" s="89" t="s">
         <v>158</v>
       </c>
       <c r="C11" s="38">
@@ -5989,17 +8218,17 @@
         <v>5000</v>
       </c>
       <c r="F11" s="54">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5000</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="100"/>
-      <c r="B12" s="101"/>
-      <c r="C12" s="100"/>
-      <c r="D12" s="100"/>
-      <c r="E12" s="102"/>
-      <c r="F12" s="102"/>
+      <c r="A12" s="86"/>
+      <c r="B12" s="87"/>
+      <c r="C12" s="86"/>
+      <c r="D12" s="86"/>
+      <c r="E12" s="88"/>
+      <c r="F12" s="88"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E13" t="s">
@@ -6007,12 +8236,12 @@
       </c>
     </row>
     <row r="17" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E17" s="98" t="s">
+      <c r="E17" s="84" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="18" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E18" s="99" t="s">
+      <c r="E18" s="85" t="s">
         <v>156</v>
       </c>
     </row>
@@ -6030,7 +8259,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6042,32 +8271,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="97" t="s">
+      <c r="A1" s="127" t="s">
         <v>153</v>
       </c>
-      <c r="B1" s="97"/>
-      <c r="C1" s="97"/>
-      <c r="D1" s="97"/>
-      <c r="E1" s="97"/>
-      <c r="F1" s="97"/>
+      <c r="B1" s="127"/>
+      <c r="C1" s="127"/>
+      <c r="D1" s="127"/>
+      <c r="E1" s="127"/>
+      <c r="F1" s="127"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="95" t="s">
+      <c r="A3" s="81" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="95" t="s">
+      <c r="B3" s="81" t="s">
         <v>91</v>
       </c>
-      <c r="C3" s="95" t="s">
+      <c r="C3" s="81" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="95" t="s">
+      <c r="D3" s="81" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="95" t="s">
+      <c r="E3" s="81" t="s">
         <v>59</v>
       </c>
-      <c r="F3" s="95" t="s">
+      <c r="F3" s="81" t="s">
         <v>11</v>
       </c>
     </row>
@@ -6089,7 +8318,7 @@
         <v>6000</v>
       </c>
       <c r="F4" s="54">
-        <f>E4*C4</f>
+        <f t="shared" ref="F4:F11" si="0">E4*C4</f>
         <v>150000</v>
       </c>
     </row>
@@ -6111,7 +8340,7 @@
         <v>6000</v>
       </c>
       <c r="F5" s="54">
-        <f>E5*C5</f>
+        <f t="shared" si="0"/>
         <v>150000</v>
       </c>
     </row>
@@ -6133,7 +8362,7 @@
         <v>6000</v>
       </c>
       <c r="F6" s="54">
-        <f>E6*C6</f>
+        <f t="shared" si="0"/>
         <v>150000</v>
       </c>
     </row>
@@ -6155,7 +8384,7 @@
         <v>16000</v>
       </c>
       <c r="F7" s="54">
-        <f>E7*C7</f>
+        <f t="shared" si="0"/>
         <v>208000</v>
       </c>
     </row>
@@ -6177,7 +8406,7 @@
         <v>6000</v>
       </c>
       <c r="F8" s="54">
-        <f>E8*C8</f>
+        <f t="shared" si="0"/>
         <v>18000</v>
       </c>
     </row>
@@ -6199,7 +8428,7 @@
         <v>11000</v>
       </c>
       <c r="F9" s="54">
-        <f>E9*C9</f>
+        <f t="shared" si="0"/>
         <v>88000</v>
       </c>
     </row>
@@ -6221,7 +8450,7 @@
         <v>41000</v>
       </c>
       <c r="F10" s="54">
-        <f>E10*C10</f>
+        <f t="shared" si="0"/>
         <v>1025000</v>
       </c>
     </row>
@@ -6243,7 +8472,7 @@
         <v>16000</v>
       </c>
       <c r="F11" s="54">
-        <f>E11*C11</f>
+        <f t="shared" si="0"/>
         <v>16000</v>
       </c>
     </row>
@@ -6261,12 +8490,12 @@
       </c>
     </row>
     <row r="18" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E18" s="98" t="s">
+      <c r="E18" s="84" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="19" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E19" s="99" t="s">
+      <c r="E19" s="85" t="s">
         <v>156</v>
       </c>
     </row>
@@ -6284,7 +8513,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6296,32 +8525,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="97" t="s">
+      <c r="A1" s="127" t="s">
         <v>153</v>
       </c>
-      <c r="B1" s="97"/>
-      <c r="C1" s="97"/>
-      <c r="D1" s="97"/>
-      <c r="E1" s="97"/>
-      <c r="F1" s="97"/>
+      <c r="B1" s="127"/>
+      <c r="C1" s="127"/>
+      <c r="D1" s="127"/>
+      <c r="E1" s="127"/>
+      <c r="F1" s="127"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="95" t="s">
+      <c r="A3" s="81" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="95" t="s">
+      <c r="B3" s="81" t="s">
         <v>91</v>
       </c>
-      <c r="C3" s="95" t="s">
+      <c r="C3" s="81" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="95" t="s">
+      <c r="D3" s="81" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="95" t="s">
+      <c r="E3" s="81" t="s">
         <v>59</v>
       </c>
-      <c r="F3" s="95" t="s">
+      <c r="F3" s="81" t="s">
         <v>11</v>
       </c>
     </row>
@@ -6343,7 +8572,7 @@
         <v>5000</v>
       </c>
       <c r="F4" s="54">
-        <f>E4*C4</f>
+        <f t="shared" ref="F4:F9" si="0">E4*C4</f>
         <v>125000</v>
       </c>
     </row>
@@ -6365,7 +8594,7 @@
         <v>5000</v>
       </c>
       <c r="F5" s="54">
-        <f>E5*C5</f>
+        <f t="shared" si="0"/>
         <v>125000</v>
       </c>
     </row>
@@ -6387,7 +8616,7 @@
         <v>15000</v>
       </c>
       <c r="F6" s="54">
-        <f>E6*C6</f>
+        <f t="shared" si="0"/>
         <v>195000</v>
       </c>
     </row>
@@ -6409,7 +8638,7 @@
         <v>5000</v>
       </c>
       <c r="F7" s="54">
-        <f>E7*C7</f>
+        <f t="shared" si="0"/>
         <v>15000</v>
       </c>
     </row>
@@ -6431,7 +8660,7 @@
         <v>10000</v>
       </c>
       <c r="F8" s="54">
-        <f>E8*C8</f>
+        <f t="shared" si="0"/>
         <v>80000</v>
       </c>
     </row>
@@ -6453,7 +8682,7 @@
         <v>15000</v>
       </c>
       <c r="F9" s="54">
-        <f>E9*C9</f>
+        <f t="shared" si="0"/>
         <v>15000</v>
       </c>
     </row>
@@ -6461,7 +8690,7 @@
       <c r="A10" s="38">
         <v>7</v>
       </c>
-      <c r="B10" s="103" t="s">
+      <c r="B10" s="89" t="s">
         <v>157</v>
       </c>
       <c r="C10" s="38">
@@ -6475,7 +8704,7 @@
         <v>200000</v>
       </c>
       <c r="F10" s="54">
-        <f t="shared" ref="F10:F11" si="0">E10*C10</f>
+        <f t="shared" ref="F10:F11" si="1">E10*C10</f>
         <v>200000</v>
       </c>
     </row>
@@ -6483,7 +8712,7 @@
       <c r="A11" s="38">
         <v>8</v>
       </c>
-      <c r="B11" s="103" t="s">
+      <c r="B11" s="89" t="s">
         <v>158</v>
       </c>
       <c r="C11" s="38">
@@ -6497,17 +8726,17 @@
         <v>5000</v>
       </c>
       <c r="F11" s="54">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5000</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="100"/>
-      <c r="B12" s="101"/>
-      <c r="C12" s="100"/>
-      <c r="D12" s="100"/>
-      <c r="E12" s="102"/>
-      <c r="F12" s="102"/>
+      <c r="A12" s="86"/>
+      <c r="B12" s="87"/>
+      <c r="C12" s="86"/>
+      <c r="D12" s="86"/>
+      <c r="E12" s="88"/>
+      <c r="F12" s="88"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E13" t="s">
@@ -6515,12 +8744,12 @@
       </c>
     </row>
     <row r="17" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E17" s="98" t="s">
+      <c r="E17" s="84" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="18" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E18" s="99" t="s">
+      <c r="E18" s="85" t="s">
         <v>156</v>
       </c>
     </row>
@@ -6535,10 +8764,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:E24"/>
+  <dimension ref="A3:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6546,26 +8775,27 @@
     <col min="2" max="2" width="18.140625" customWidth="1"/>
     <col min="3" max="3" width="10.140625" customWidth="1"/>
     <col min="4" max="5" width="11.5703125" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="95" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="81" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="95" t="s">
+      <c r="B3" s="81" t="s">
         <v>198</v>
       </c>
-      <c r="C3" s="95" t="s">
+      <c r="C3" s="81" t="s">
         <v>165</v>
       </c>
-      <c r="D3" s="95" t="s">
+      <c r="D3" s="81" t="s">
         <v>171</v>
       </c>
-      <c r="E3" s="95" t="s">
+      <c r="E3" s="81" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="38">
         <v>1</v>
       </c>
@@ -6575,16 +8805,25 @@
       <c r="C4" s="38" t="s">
         <v>159</v>
       </c>
-      <c r="D4" s="38" t="e">
-        <f>HLOOKUP(C4, 'daftar harga'!#REF!,2)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="E4" s="38" t="e">
-        <f>HLOOKUP(C4, 'daftar harga'!#REF!,2)</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D4" s="38" t="str">
+        <f>VLOOKUP(C4,$H$4:$J$10,2)</f>
+        <v>Olahraga</v>
+      </c>
+      <c r="E4" s="38" t="str">
+        <f>VLOOKUP(C4,$I$4:$J$10,1)</f>
+        <v>Olahraga</v>
+      </c>
+      <c r="H4" s="81" t="s">
+        <v>165</v>
+      </c>
+      <c r="I4" s="81" t="s">
+        <v>171</v>
+      </c>
+      <c r="J4" s="81" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="38">
         <v>2</v>
       </c>
@@ -6594,16 +8833,25 @@
       <c r="C5" s="38" t="s">
         <v>160</v>
       </c>
-      <c r="D5" s="38" t="e">
-        <f>HLOOKUP(C5, 'daftar harga'!#REF!,2)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="E5" s="38" t="e">
-        <f>HLOOKUP(C5, 'daftar harga'!#REF!,2)</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D5" s="38" t="str">
+        <f t="shared" ref="D5:D24" si="0">VLOOKUP(C5,$H$4:$J$10,2)</f>
+        <v>Olahraga</v>
+      </c>
+      <c r="E5" s="38" t="str">
+        <f t="shared" ref="E5:E24" si="1">VLOOKUP(C5,$I$4:$J$10,1)</f>
+        <v>Olahraga</v>
+      </c>
+      <c r="H5" s="38" t="s">
+        <v>159</v>
+      </c>
+      <c r="I5" s="38" t="s">
+        <v>166</v>
+      </c>
+      <c r="J5" s="38" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="38">
         <v>3</v>
       </c>
@@ -6613,16 +8861,25 @@
       <c r="C6" s="38" t="s">
         <v>159</v>
       </c>
-      <c r="D6" s="38" t="e">
-        <f>HLOOKUP(C6, 'daftar harga'!#REF!,2)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="E6" s="38" t="e">
-        <f>HLOOKUP(C6, 'daftar harga'!#REF!,2)</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D6" s="38" t="str">
+        <f t="shared" si="0"/>
+        <v>Olahraga</v>
+      </c>
+      <c r="E6" s="38" t="str">
+        <f t="shared" si="1"/>
+        <v>Olahraga</v>
+      </c>
+      <c r="H6" s="38" t="s">
+        <v>160</v>
+      </c>
+      <c r="I6" s="38" t="s">
+        <v>166</v>
+      </c>
+      <c r="J6" s="38" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="38">
         <v>4</v>
       </c>
@@ -6632,16 +8889,25 @@
       <c r="C7" s="38" t="s">
         <v>163</v>
       </c>
-      <c r="D7" s="38" t="e">
-        <f>HLOOKUP(C7, 'daftar harga'!#REF!,2)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="E7" s="38" t="e">
-        <f>HLOOKUP(C7, 'daftar harga'!#REF!,2)</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D7" s="38" t="str">
+        <f t="shared" si="0"/>
+        <v>Baju Siswa</v>
+      </c>
+      <c r="E7" s="38" t="str">
+        <f t="shared" si="1"/>
+        <v>Batik</v>
+      </c>
+      <c r="H7" s="38" t="s">
+        <v>161</v>
+      </c>
+      <c r="I7" s="38" t="s">
+        <v>167</v>
+      </c>
+      <c r="J7" s="38" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="38">
         <v>5</v>
       </c>
@@ -6651,16 +8917,25 @@
       <c r="C8" s="38" t="s">
         <v>160</v>
       </c>
-      <c r="D8" s="38" t="e">
-        <f>HLOOKUP(C8, 'daftar harga'!#REF!,2)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="E8" s="38" t="e">
-        <f>HLOOKUP(C8, 'daftar harga'!#REF!,2)</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D8" s="38" t="str">
+        <f t="shared" si="0"/>
+        <v>Olahraga</v>
+      </c>
+      <c r="E8" s="38" t="str">
+        <f t="shared" si="1"/>
+        <v>Olahraga</v>
+      </c>
+      <c r="H8" s="38" t="s">
+        <v>162</v>
+      </c>
+      <c r="I8" s="38" t="s">
+        <v>168</v>
+      </c>
+      <c r="J8" s="38" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="38">
         <v>6</v>
       </c>
@@ -6670,16 +8945,25 @@
       <c r="C9" s="38" t="s">
         <v>159</v>
       </c>
-      <c r="D9" s="38" t="e">
-        <f>HLOOKUP(C9, 'daftar harga'!#REF!,2)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="E9" s="38" t="e">
-        <f>HLOOKUP(C9, 'daftar harga'!#REF!,2)</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D9" s="38" t="str">
+        <f t="shared" si="0"/>
+        <v>Olahraga</v>
+      </c>
+      <c r="E9" s="38" t="str">
+        <f t="shared" si="1"/>
+        <v>Olahraga</v>
+      </c>
+      <c r="H9" s="38" t="s">
+        <v>163</v>
+      </c>
+      <c r="I9" s="38" t="s">
+        <v>169</v>
+      </c>
+      <c r="J9" s="38" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="38">
         <v>7</v>
       </c>
@@ -6689,16 +8973,25 @@
       <c r="C10" s="38" t="s">
         <v>160</v>
       </c>
-      <c r="D10" s="38" t="e">
-        <f>HLOOKUP(C10, 'daftar harga'!#REF!,2)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="E10" s="38" t="e">
-        <f>HLOOKUP(C10, 'daftar harga'!#REF!,2)</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D10" s="38" t="str">
+        <f t="shared" si="0"/>
+        <v>Olahraga</v>
+      </c>
+      <c r="E10" s="38" t="str">
+        <f t="shared" si="1"/>
+        <v>Olahraga</v>
+      </c>
+      <c r="H10" s="38" t="s">
+        <v>164</v>
+      </c>
+      <c r="I10" s="38" t="s">
+        <v>170</v>
+      </c>
+      <c r="J10" s="38" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="38">
         <v>8</v>
       </c>
@@ -6708,16 +9001,16 @@
       <c r="C11" s="38" t="s">
         <v>162</v>
       </c>
-      <c r="D11" s="38" t="e">
-        <f>HLOOKUP(C11, 'daftar harga'!#REF!,2)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="E11" s="38" t="e">
-        <f>HLOOKUP(C11, 'daftar harga'!#REF!,2)</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D11" s="38" t="str">
+        <f t="shared" si="0"/>
+        <v>Baju Siswa</v>
+      </c>
+      <c r="E11" s="38" t="str">
+        <f t="shared" si="1"/>
+        <v>Batik</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="38">
         <v>9</v>
       </c>
@@ -6727,16 +9020,16 @@
       <c r="C12" s="38" t="s">
         <v>163</v>
       </c>
-      <c r="D12" s="38" t="e">
-        <f>HLOOKUP(C12, 'daftar harga'!#REF!,2)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="E12" s="38" t="e">
-        <f>HLOOKUP(C12, 'daftar harga'!#REF!,2)</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D12" s="38" t="str">
+        <f t="shared" si="0"/>
+        <v>Baju Siswa</v>
+      </c>
+      <c r="E12" s="38" t="str">
+        <f t="shared" si="1"/>
+        <v>Batik</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="38">
         <v>10</v>
       </c>
@@ -6746,16 +9039,16 @@
       <c r="C13" s="38" t="s">
         <v>161</v>
       </c>
-      <c r="D13" s="38" t="e">
-        <f>HLOOKUP(C13, 'daftar harga'!#REF!,2)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="E13" s="38" t="e">
-        <f>HLOOKUP(C13, 'daftar harga'!#REF!,2)</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D13" s="38" t="str">
+        <f t="shared" si="0"/>
+        <v>Batik</v>
+      </c>
+      <c r="E13" s="38" t="str">
+        <f t="shared" si="1"/>
+        <v>Olahraga</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="38">
         <v>11</v>
       </c>
@@ -6765,16 +9058,16 @@
       <c r="C14" s="38" t="s">
         <v>163</v>
       </c>
-      <c r="D14" s="38" t="e">
-        <f>HLOOKUP(C14, 'daftar harga'!#REF!,2)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="E14" s="38" t="e">
-        <f>HLOOKUP(C14, 'daftar harga'!#REF!,2)</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D14" s="38" t="str">
+        <f t="shared" si="0"/>
+        <v>Baju Siswa</v>
+      </c>
+      <c r="E14" s="38" t="str">
+        <f t="shared" si="1"/>
+        <v>Batik</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="38">
         <v>12</v>
       </c>
@@ -6784,16 +9077,16 @@
       <c r="C15" s="38" t="s">
         <v>163</v>
       </c>
-      <c r="D15" s="38" t="e">
-        <f>HLOOKUP(C15, 'daftar harga'!#REF!,2)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="E15" s="38" t="e">
-        <f>HLOOKUP(C15, 'daftar harga'!#REF!,2)</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D15" s="38" t="str">
+        <f t="shared" si="0"/>
+        <v>Baju Siswa</v>
+      </c>
+      <c r="E15" s="38" t="str">
+        <f t="shared" si="1"/>
+        <v>Batik</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="38">
         <v>13</v>
       </c>
@@ -6803,13 +9096,13 @@
       <c r="C16" s="38" t="s">
         <v>161</v>
       </c>
-      <c r="D16" s="38" t="e">
-        <f>HLOOKUP(C16, 'daftar harga'!#REF!,2)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="E16" s="38" t="e">
-        <f>HLOOKUP(C16, 'daftar harga'!#REF!,2)</f>
-        <v>#REF!</v>
+      <c r="D16" s="38" t="str">
+        <f t="shared" si="0"/>
+        <v>Batik</v>
+      </c>
+      <c r="E16" s="38" t="str">
+        <f t="shared" si="1"/>
+        <v>Olahraga</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -6822,13 +9115,13 @@
       <c r="C17" s="38" t="s">
         <v>160</v>
       </c>
-      <c r="D17" s="38" t="e">
-        <f>HLOOKUP(C17, 'daftar harga'!#REF!,2)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="E17" s="38" t="e">
-        <f>HLOOKUP(C17, 'daftar harga'!#REF!,2)</f>
-        <v>#REF!</v>
+      <c r="D17" s="38" t="str">
+        <f t="shared" si="0"/>
+        <v>Olahraga</v>
+      </c>
+      <c r="E17" s="38" t="str">
+        <f t="shared" si="1"/>
+        <v>Olahraga</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -6841,13 +9134,13 @@
       <c r="C18" s="38" t="s">
         <v>164</v>
       </c>
-      <c r="D18" s="38" t="e">
-        <f>HLOOKUP(C18, 'daftar harga'!#REF!,2)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="E18" s="38" t="e">
-        <f>HLOOKUP(C18, 'daftar harga'!#REF!,2)</f>
-        <v>#REF!</v>
+      <c r="D18" s="38" t="str">
+        <f t="shared" si="0"/>
+        <v>Olahraga</v>
+      </c>
+      <c r="E18" s="38" t="str">
+        <f t="shared" si="1"/>
+        <v>Olahraga</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -6860,13 +9153,13 @@
       <c r="C19" s="38" t="s">
         <v>163</v>
       </c>
-      <c r="D19" s="38" t="e">
-        <f>HLOOKUP(C19, 'daftar harga'!#REF!,2)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="E19" s="38" t="e">
-        <f>HLOOKUP(C19, 'daftar harga'!#REF!,2)</f>
-        <v>#REF!</v>
+      <c r="D19" s="38" t="str">
+        <f t="shared" si="0"/>
+        <v>Baju Siswa</v>
+      </c>
+      <c r="E19" s="38" t="str">
+        <f t="shared" si="1"/>
+        <v>Batik</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -6879,13 +9172,13 @@
       <c r="C20" s="38" t="s">
         <v>160</v>
       </c>
-      <c r="D20" s="38" t="e">
-        <f>HLOOKUP(C20, 'daftar harga'!#REF!,2)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="E20" s="38" t="e">
-        <f>HLOOKUP(C20, 'daftar harga'!#REF!,2)</f>
-        <v>#REF!</v>
+      <c r="D20" s="38" t="str">
+        <f t="shared" si="0"/>
+        <v>Olahraga</v>
+      </c>
+      <c r="E20" s="38" t="str">
+        <f t="shared" si="1"/>
+        <v>Olahraga</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -6898,13 +9191,13 @@
       <c r="C21" s="38" t="s">
         <v>159</v>
       </c>
-      <c r="D21" s="38" t="e">
-        <f>HLOOKUP(C21, 'daftar harga'!#REF!,2)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="E21" s="38" t="e">
-        <f>HLOOKUP(C21, 'daftar harga'!#REF!,2)</f>
-        <v>#REF!</v>
+      <c r="D21" s="38" t="str">
+        <f t="shared" si="0"/>
+        <v>Olahraga</v>
+      </c>
+      <c r="E21" s="38" t="str">
+        <f t="shared" si="1"/>
+        <v>Olahraga</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -6917,13 +9210,13 @@
       <c r="C22" s="38" t="s">
         <v>160</v>
       </c>
-      <c r="D22" s="38" t="e">
-        <f>HLOOKUP(C22, 'daftar harga'!#REF!,2)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="E22" s="38" t="e">
-        <f>HLOOKUP(C22, 'daftar harga'!#REF!,2)</f>
-        <v>#REF!</v>
+      <c r="D22" s="38" t="str">
+        <f t="shared" si="0"/>
+        <v>Olahraga</v>
+      </c>
+      <c r="E22" s="38" t="str">
+        <f t="shared" si="1"/>
+        <v>Olahraga</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -6936,13 +9229,13 @@
       <c r="C23" s="38" t="s">
         <v>163</v>
       </c>
-      <c r="D23" s="38" t="e">
-        <f>HLOOKUP(C23, 'daftar harga'!#REF!,2)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="E23" s="38" t="e">
-        <f>HLOOKUP(C23, 'daftar harga'!#REF!,2)</f>
-        <v>#REF!</v>
+      <c r="D23" s="38" t="str">
+        <f t="shared" si="0"/>
+        <v>Baju Siswa</v>
+      </c>
+      <c r="E23" s="38" t="str">
+        <f t="shared" si="1"/>
+        <v>Batik</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -6955,13 +9248,13 @@
       <c r="C24" s="38" t="s">
         <v>160</v>
       </c>
-      <c r="D24" s="38" t="e">
-        <f>HLOOKUP(C24, 'daftar harga'!#REF!,2)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="E24" s="38" t="e">
-        <f>HLOOKUP(C24, 'daftar harga'!#REF!,2)</f>
-        <v>#REF!</v>
+      <c r="D24" s="38" t="str">
+        <f t="shared" si="0"/>
+        <v>Olahraga</v>
+      </c>
+      <c r="E24" s="38" t="str">
+        <f t="shared" si="1"/>
+        <v>Olahraga</v>
       </c>
     </row>
   </sheetData>

</xml_diff>